<commit_message>
Fitur Cuti, Plugin Excel dan PDF sudah selesai
</commit_message>
<xml_diff>
--- a/assets/excel/Daftar Pegawai.xlsx
+++ b/assets/excel/Daftar Pegawai.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Daftar Pegawai" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
@@ -524,10 +524,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -835,7 +832,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -1710,7 +1707,7 @@
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>
@@ -1719,5 +1716,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new excel admin fix
</commit_message>
<xml_diff>
--- a/assets/excel/Daftar Pegawai.xlsx
+++ b/assets/excel/Daftar Pegawai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="170">
   <si>
     <t>DAFTAR PEGAWAI</t>
   </si>
@@ -501,6 +501,30 @@
   </si>
   <si>
     <t>2080-04-27</t>
+  </si>
+  <si>
+    <t>M Safroni</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>2000-07-13</t>
+  </si>
+  <si>
+    <t>jakarta pusat</t>
+  </si>
+  <si>
+    <t>082180712764</t>
+  </si>
+  <si>
+    <t>apalah@gmail.com</t>
+  </si>
+  <si>
+    <t>Cetak</t>
+  </si>
+  <si>
+    <t>2058-07-13</t>
   </si>
 </sst>
 </file>
@@ -836,7 +860,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1701,6 +1725,60 @@
       </c>
       <c r="T16" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>1789621</v>
+      </c>
+      <c r="D17" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" t="s">
+        <v>164</v>
+      </c>
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" t="s">
+        <v>154</v>
+      </c>
+      <c r="K17" t="s">
+        <v>155</v>
+      </c>
+      <c r="L17" t="s">
+        <v>165</v>
+      </c>
+      <c r="M17" t="s">
+        <v>166</v>
+      </c>
+      <c r="N17" t="s">
+        <v>167</v>
+      </c>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17" t="s">
+        <v>168</v>
+      </c>
+      <c r="T17" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data pegawai, pencarian, sebagian history, ganti password
</commit_message>
<xml_diff>
--- a/assets/excel/Daftar Pegawai.xlsx
+++ b/assets/excel/Daftar Pegawai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="295">
   <si>
     <t>DAFTAR PEGAWAI</t>
   </si>
@@ -873,6 +873,33 @@
   </si>
   <si>
     <t>Pradita Ferani</t>
+  </si>
+  <si>
+    <t>Burhanu Sultan Ramadan</t>
+  </si>
+  <si>
+    <t>Darit</t>
+  </si>
+  <si>
+    <t>2001-08-09</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>Belum Menikah</t>
+  </si>
+  <si>
+    <t>2059-08-09</t>
+  </si>
+  <si>
+    <t>Jawhead</t>
+  </si>
+  <si>
+    <t>Badang</t>
+  </si>
+  <si>
+    <t>A-</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1235,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R167"/>
+  <dimension ref="A1:R170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -7418,6 +7445,138 @@
       <c r="P167"/>
       <c r="Q167"/>
       <c r="R167"/>
+    </row>
+    <row r="168" spans="1:18">
+      <c r="A168">
+        <v>165</v>
+      </c>
+      <c r="B168">
+        <v>165</v>
+      </c>
+      <c r="C168">
+        <v>52635235235</v>
+      </c>
+      <c r="D168" t="s">
+        <v>286</v>
+      </c>
+      <c r="E168" t="s">
+        <v>287</v>
+      </c>
+      <c r="F168" t="s">
+        <v>288</v>
+      </c>
+      <c r="G168" t="s">
+        <v>21</v>
+      </c>
+      <c r="H168" t="s">
+        <v>22</v>
+      </c>
+      <c r="I168" t="s">
+        <v>289</v>
+      </c>
+      <c r="J168" t="s">
+        <v>290</v>
+      </c>
+      <c r="K168" t="s">
+        <v>25</v>
+      </c>
+      <c r="L168"/>
+      <c r="M168"/>
+      <c r="N168"/>
+      <c r="O168"/>
+      <c r="P168"/>
+      <c r="Q168"/>
+      <c r="R168" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18">
+      <c r="A169">
+        <v>166</v>
+      </c>
+      <c r="B169">
+        <v>166</v>
+      </c>
+      <c r="C169">
+        <v>123456</v>
+      </c>
+      <c r="D169" t="s">
+        <v>292</v>
+      </c>
+      <c r="E169" t="s">
+        <v>287</v>
+      </c>
+      <c r="F169" t="s">
+        <v>288</v>
+      </c>
+      <c r="G169" t="s">
+        <v>21</v>
+      </c>
+      <c r="H169" t="s">
+        <v>22</v>
+      </c>
+      <c r="I169" t="s">
+        <v>23</v>
+      </c>
+      <c r="J169" t="s">
+        <v>24</v>
+      </c>
+      <c r="K169" t="s">
+        <v>25</v>
+      </c>
+      <c r="L169"/>
+      <c r="M169"/>
+      <c r="N169"/>
+      <c r="O169"/>
+      <c r="P169"/>
+      <c r="Q169"/>
+      <c r="R169" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18">
+      <c r="A170">
+        <v>167</v>
+      </c>
+      <c r="B170">
+        <v>167</v>
+      </c>
+      <c r="C170">
+        <v>1234567890</v>
+      </c>
+      <c r="D170" t="s">
+        <v>293</v>
+      </c>
+      <c r="E170" t="s">
+        <v>287</v>
+      </c>
+      <c r="F170" t="s">
+        <v>288</v>
+      </c>
+      <c r="G170" t="s">
+        <v>21</v>
+      </c>
+      <c r="H170" t="s">
+        <v>22</v>
+      </c>
+      <c r="I170" t="s">
+        <v>294</v>
+      </c>
+      <c r="J170" t="s">
+        <v>24</v>
+      </c>
+      <c r="K170" t="s">
+        <v>25</v>
+      </c>
+      <c r="L170"/>
+      <c r="M170"/>
+      <c r="N170"/>
+      <c r="O170"/>
+      <c r="P170"/>
+      <c r="Q170"/>
+      <c r="R170" t="s">
+        <v>291</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
menambah tanggal resign di data pegawai
</commit_message>
<xml_diff>
--- a/assets/excel/Daftar Pegawai.xlsx
+++ b/assets/excel/Daftar Pegawai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="292">
   <si>
     <t>DAFTAR PEGAWAI</t>
   </si>
@@ -884,22 +884,13 @@
     <t>2001-08-09</t>
   </si>
   <si>
-    <t>B+</t>
+    <t>A-</t>
   </si>
   <si>
     <t>Belum Menikah</t>
   </si>
   <si>
     <t>2059-08-09</t>
-  </si>
-  <si>
-    <t>Jawhead</t>
-  </si>
-  <si>
-    <t>Badang</t>
-  </si>
-  <si>
-    <t>A-</t>
   </si>
 </sst>
 </file>
@@ -1235,7 +1226,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R170"/>
+  <dimension ref="A1:R168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -7454,7 +7445,7 @@
         <v>165</v>
       </c>
       <c r="C168">
-        <v>52635235235</v>
+        <v>9535253</v>
       </c>
       <c r="D168" t="s">
         <v>286</v>
@@ -7487,94 +7478,6 @@
       <c r="P168"/>
       <c r="Q168"/>
       <c r="R168" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="169" spans="1:18">
-      <c r="A169">
-        <v>166</v>
-      </c>
-      <c r="B169">
-        <v>166</v>
-      </c>
-      <c r="C169">
-        <v>123456</v>
-      </c>
-      <c r="D169" t="s">
-        <v>292</v>
-      </c>
-      <c r="E169" t="s">
-        <v>287</v>
-      </c>
-      <c r="F169" t="s">
-        <v>288</v>
-      </c>
-      <c r="G169" t="s">
-        <v>21</v>
-      </c>
-      <c r="H169" t="s">
-        <v>22</v>
-      </c>
-      <c r="I169" t="s">
-        <v>23</v>
-      </c>
-      <c r="J169" t="s">
-        <v>24</v>
-      </c>
-      <c r="K169" t="s">
-        <v>25</v>
-      </c>
-      <c r="L169"/>
-      <c r="M169"/>
-      <c r="N169"/>
-      <c r="O169"/>
-      <c r="P169"/>
-      <c r="Q169"/>
-      <c r="R169" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="170" spans="1:18">
-      <c r="A170">
-        <v>167</v>
-      </c>
-      <c r="B170">
-        <v>167</v>
-      </c>
-      <c r="C170">
-        <v>1234567890</v>
-      </c>
-      <c r="D170" t="s">
-        <v>293</v>
-      </c>
-      <c r="E170" t="s">
-        <v>287</v>
-      </c>
-      <c r="F170" t="s">
-        <v>288</v>
-      </c>
-      <c r="G170" t="s">
-        <v>21</v>
-      </c>
-      <c r="H170" t="s">
-        <v>22</v>
-      </c>
-      <c r="I170" t="s">
-        <v>294</v>
-      </c>
-      <c r="J170" t="s">
-        <v>24</v>
-      </c>
-      <c r="K170" t="s">
-        <v>25</v>
-      </c>
-      <c r="L170"/>
-      <c r="M170"/>
-      <c r="N170"/>
-      <c r="O170"/>
-      <c r="P170"/>
-      <c r="Q170"/>
-      <c r="R170" t="s">
         <v>291</v>
       </c>
     </row>

</xml_diff>

<commit_message>
perbaikan pada baris ttl pegawai, dan penambahan tombol unset jabatan aktif
</commit_message>
<xml_diff>
--- a/assets/excel/Daftar Pegawai.xlsx
+++ b/assets/excel/Daftar Pegawai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="294">
   <si>
     <t>DAFTAR PEGAWAI</t>
   </si>
@@ -239,6 +239,9 @@
     <t>Kanang Suhartanto</t>
   </si>
   <si>
+    <t>Non-Aktif</t>
+  </si>
+  <si>
     <t>2012.12.04.035</t>
   </si>
   <si>
@@ -684,6 +687,9 @@
   </si>
   <si>
     <t>YUSUF PURNAMA</t>
+  </si>
+  <si>
+    <t>Berhenti</t>
   </si>
   <si>
     <t>AKHMAD RIFAI</t>
@@ -2235,7 +2241,7 @@
         <v>24</v>
       </c>
       <c r="K28" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L28"/>
       <c r="M28"/>
@@ -2253,10 +2259,10 @@
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E29"/>
       <c r="F29"/>
@@ -2291,10 +2297,10 @@
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E30"/>
       <c r="F30"/>
@@ -2311,7 +2317,7 @@
         <v>24</v>
       </c>
       <c r="K30" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L30"/>
       <c r="M30"/>
@@ -2329,10 +2335,10 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E31"/>
       <c r="F31"/>
@@ -2367,10 +2373,10 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E32"/>
       <c r="F32"/>
@@ -2405,10 +2411,10 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E33"/>
       <c r="F33"/>
@@ -2443,10 +2449,10 @@
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E34"/>
       <c r="F34"/>
@@ -2481,10 +2487,10 @@
         <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D35" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E35"/>
       <c r="F35"/>
@@ -2519,10 +2525,10 @@
         <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E36"/>
       <c r="F36"/>
@@ -2557,10 +2563,10 @@
         <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E37"/>
       <c r="F37"/>
@@ -2595,10 +2601,10 @@
         <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D38" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E38"/>
       <c r="F38"/>
@@ -2633,10 +2639,10 @@
         <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D39" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E39"/>
       <c r="F39"/>
@@ -2671,10 +2677,10 @@
         <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D40" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E40"/>
       <c r="F40"/>
@@ -2709,10 +2715,10 @@
         <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E41"/>
       <c r="F41"/>
@@ -2747,10 +2753,10 @@
         <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D42" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E42"/>
       <c r="F42"/>
@@ -2785,10 +2791,10 @@
         <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D43" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E43"/>
       <c r="F43"/>
@@ -2823,10 +2829,10 @@
         <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D44" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E44"/>
       <c r="F44"/>
@@ -2861,10 +2867,10 @@
         <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D45" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E45"/>
       <c r="F45"/>
@@ -2899,10 +2905,10 @@
         <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D46" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E46"/>
       <c r="F46"/>
@@ -2937,10 +2943,10 @@
         <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D47" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E47"/>
       <c r="F47"/>
@@ -2975,10 +2981,10 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D48" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E48"/>
       <c r="F48"/>
@@ -3013,10 +3019,10 @@
         <v>46</v>
       </c>
       <c r="C49" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D49" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E49"/>
       <c r="F49"/>
@@ -3051,10 +3057,10 @@
         <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D50" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E50"/>
       <c r="F50"/>
@@ -3089,10 +3095,10 @@
         <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D51" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E51"/>
       <c r="F51"/>
@@ -3127,10 +3133,10 @@
         <v>49</v>
       </c>
       <c r="C52" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D52" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E52"/>
       <c r="F52"/>
@@ -3165,10 +3171,10 @@
         <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D53" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E53"/>
       <c r="F53"/>
@@ -3203,10 +3209,10 @@
         <v>51</v>
       </c>
       <c r="C54" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D54" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E54"/>
       <c r="F54"/>
@@ -3241,10 +3247,10 @@
         <v>52</v>
       </c>
       <c r="C55" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D55" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E55"/>
       <c r="F55"/>
@@ -3261,7 +3267,7 @@
         <v>24</v>
       </c>
       <c r="K55" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L55"/>
       <c r="M55"/>
@@ -3279,10 +3285,10 @@
         <v>53</v>
       </c>
       <c r="C56" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D56" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E56"/>
       <c r="F56"/>
@@ -3317,10 +3323,10 @@
         <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D57" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E57"/>
       <c r="F57"/>
@@ -3355,10 +3361,10 @@
         <v>55</v>
       </c>
       <c r="C58" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D58" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E58"/>
       <c r="F58"/>
@@ -3393,10 +3399,10 @@
         <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D59" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E59"/>
       <c r="F59"/>
@@ -3431,10 +3437,10 @@
         <v>57</v>
       </c>
       <c r="C60" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D60" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E60"/>
       <c r="F60"/>
@@ -3469,10 +3475,10 @@
         <v>58</v>
       </c>
       <c r="C61" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D61" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E61"/>
       <c r="F61"/>
@@ -3507,10 +3513,10 @@
         <v>59</v>
       </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D62" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E62"/>
       <c r="F62"/>
@@ -3545,10 +3551,10 @@
         <v>60</v>
       </c>
       <c r="C63" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D63" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E63"/>
       <c r="F63"/>
@@ -3565,7 +3571,7 @@
         <v>24</v>
       </c>
       <c r="K63" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L63"/>
       <c r="M63"/>
@@ -3583,10 +3589,10 @@
         <v>61</v>
       </c>
       <c r="C64" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D64" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E64"/>
       <c r="F64"/>
@@ -3621,10 +3627,10 @@
         <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D65" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E65"/>
       <c r="F65"/>
@@ -3659,10 +3665,10 @@
         <v>63</v>
       </c>
       <c r="C66" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D66" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E66"/>
       <c r="F66"/>
@@ -3697,10 +3703,10 @@
         <v>64</v>
       </c>
       <c r="C67" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D67" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E67"/>
       <c r="F67"/>
@@ -3735,10 +3741,10 @@
         <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D68" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E68"/>
       <c r="F68"/>
@@ -3773,10 +3779,10 @@
         <v>66</v>
       </c>
       <c r="C69" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D69" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E69"/>
       <c r="F69"/>
@@ -3811,10 +3817,10 @@
         <v>67</v>
       </c>
       <c r="C70" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D70" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E70"/>
       <c r="F70"/>
@@ -3849,10 +3855,10 @@
         <v>68</v>
       </c>
       <c r="C71" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D71" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E71"/>
       <c r="F71"/>
@@ -3887,10 +3893,10 @@
         <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D72" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E72"/>
       <c r="F72"/>
@@ -3925,10 +3931,10 @@
         <v>70</v>
       </c>
       <c r="C73" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D73" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E73"/>
       <c r="F73"/>
@@ -3945,7 +3951,7 @@
         <v>24</v>
       </c>
       <c r="K73" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L73"/>
       <c r="M73"/>
@@ -3963,10 +3969,10 @@
         <v>71</v>
       </c>
       <c r="C74" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D74" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E74"/>
       <c r="F74"/>
@@ -4001,10 +4007,10 @@
         <v>72</v>
       </c>
       <c r="C75" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D75" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E75"/>
       <c r="F75"/>
@@ -4021,7 +4027,7 @@
         <v>24</v>
       </c>
       <c r="K75" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L75"/>
       <c r="M75"/>
@@ -4039,10 +4045,10 @@
         <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D76" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E76"/>
       <c r="F76"/>
@@ -4059,7 +4065,7 @@
         <v>24</v>
       </c>
       <c r="K76" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L76"/>
       <c r="M76"/>
@@ -4077,10 +4083,10 @@
         <v>74</v>
       </c>
       <c r="C77" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D77" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E77"/>
       <c r="F77"/>
@@ -4097,7 +4103,7 @@
         <v>24</v>
       </c>
       <c r="K77" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L77"/>
       <c r="M77"/>
@@ -4115,10 +4121,10 @@
         <v>75</v>
       </c>
       <c r="C78" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D78" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E78"/>
       <c r="F78"/>
@@ -4153,10 +4159,10 @@
         <v>76</v>
       </c>
       <c r="C79" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D79" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E79"/>
       <c r="F79"/>
@@ -4191,10 +4197,10 @@
         <v>77</v>
       </c>
       <c r="C80" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D80" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E80"/>
       <c r="F80"/>
@@ -4229,10 +4235,10 @@
         <v>78</v>
       </c>
       <c r="C81" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D81" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E81"/>
       <c r="F81"/>
@@ -4267,10 +4273,10 @@
         <v>79</v>
       </c>
       <c r="C82" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D82" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E82"/>
       <c r="F82"/>
@@ -4287,7 +4293,7 @@
         <v>24</v>
       </c>
       <c r="K82" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L82"/>
       <c r="M82"/>
@@ -4305,10 +4311,10 @@
         <v>80</v>
       </c>
       <c r="C83" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D83" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E83"/>
       <c r="F83"/>
@@ -4343,10 +4349,10 @@
         <v>81</v>
       </c>
       <c r="C84" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D84" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E84"/>
       <c r="F84"/>
@@ -4363,7 +4369,7 @@
         <v>24</v>
       </c>
       <c r="K84" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L84"/>
       <c r="M84"/>
@@ -4381,10 +4387,10 @@
         <v>82</v>
       </c>
       <c r="C85" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D85" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E85"/>
       <c r="F85"/>
@@ -4419,10 +4425,10 @@
         <v>83</v>
       </c>
       <c r="C86" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D86" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E86"/>
       <c r="F86"/>
@@ -4439,7 +4445,7 @@
         <v>24</v>
       </c>
       <c r="K86" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L86"/>
       <c r="M86"/>
@@ -4457,10 +4463,10 @@
         <v>84</v>
       </c>
       <c r="C87" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D87" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E87"/>
       <c r="F87"/>
@@ -4477,7 +4483,7 @@
         <v>24</v>
       </c>
       <c r="K87" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L87"/>
       <c r="M87"/>
@@ -4495,10 +4501,10 @@
         <v>85</v>
       </c>
       <c r="C88" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D88" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E88"/>
       <c r="F88"/>
@@ -4533,10 +4539,10 @@
         <v>86</v>
       </c>
       <c r="C89" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D89" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E89"/>
       <c r="F89"/>
@@ -4553,7 +4559,7 @@
         <v>24</v>
       </c>
       <c r="K89" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L89"/>
       <c r="M89"/>
@@ -4571,10 +4577,10 @@
         <v>87</v>
       </c>
       <c r="C90" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D90" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E90"/>
       <c r="F90"/>
@@ -4609,10 +4615,10 @@
         <v>88</v>
       </c>
       <c r="C91" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D91" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E91"/>
       <c r="F91"/>
@@ -4647,10 +4653,10 @@
         <v>89</v>
       </c>
       <c r="C92" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D92" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E92"/>
       <c r="F92"/>
@@ -4685,10 +4691,10 @@
         <v>90</v>
       </c>
       <c r="C93" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D93" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E93"/>
       <c r="F93"/>
@@ -4705,7 +4711,7 @@
         <v>24</v>
       </c>
       <c r="K93" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L93"/>
       <c r="M93"/>
@@ -4723,10 +4729,10 @@
         <v>91</v>
       </c>
       <c r="C94" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D94" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E94"/>
       <c r="F94"/>
@@ -4761,10 +4767,10 @@
         <v>92</v>
       </c>
       <c r="C95" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D95" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E95"/>
       <c r="F95"/>
@@ -4781,7 +4787,7 @@
         <v>24</v>
       </c>
       <c r="K95" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L95"/>
       <c r="M95"/>
@@ -4799,10 +4805,10 @@
         <v>93</v>
       </c>
       <c r="C96" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D96" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E96"/>
       <c r="F96"/>
@@ -4837,10 +4843,10 @@
         <v>94</v>
       </c>
       <c r="C97" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D97" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E97"/>
       <c r="F97"/>
@@ -4875,10 +4881,10 @@
         <v>95</v>
       </c>
       <c r="C98" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D98" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E98"/>
       <c r="F98"/>
@@ -4913,10 +4919,10 @@
         <v>96</v>
       </c>
       <c r="C99" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D99" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E99"/>
       <c r="F99"/>
@@ -4951,10 +4957,10 @@
         <v>97</v>
       </c>
       <c r="C100" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D100" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E100"/>
       <c r="F100"/>
@@ -4989,10 +4995,10 @@
         <v>98</v>
       </c>
       <c r="C101" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D101" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E101"/>
       <c r="F101"/>
@@ -5027,10 +5033,10 @@
         <v>99</v>
       </c>
       <c r="C102" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D102" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E102"/>
       <c r="F102"/>
@@ -5068,7 +5074,7 @@
         <v>1000</v>
       </c>
       <c r="D103" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E103"/>
       <c r="F103"/>
@@ -5085,7 +5091,7 @@
         <v>24</v>
       </c>
       <c r="K103" t="s">
-        <v>25</v>
+        <v>224</v>
       </c>
       <c r="L103"/>
       <c r="M103"/>
@@ -5106,7 +5112,7 @@
         <v>1001</v>
       </c>
       <c r="D104" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E104"/>
       <c r="F104"/>
@@ -5123,7 +5129,7 @@
         <v>24</v>
       </c>
       <c r="K104" t="s">
-        <v>25</v>
+        <v>224</v>
       </c>
       <c r="L104"/>
       <c r="M104"/>
@@ -5144,7 +5150,7 @@
         <v>1002</v>
       </c>
       <c r="D105" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E105"/>
       <c r="F105"/>
@@ -5182,7 +5188,7 @@
         <v>1003</v>
       </c>
       <c r="D106" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E106"/>
       <c r="F106"/>
@@ -5199,7 +5205,7 @@
         <v>24</v>
       </c>
       <c r="K106" t="s">
-        <v>25</v>
+        <v>224</v>
       </c>
       <c r="L106"/>
       <c r="M106"/>
@@ -5220,7 +5226,7 @@
         <v>2000</v>
       </c>
       <c r="D107" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E107"/>
       <c r="F107"/>
@@ -5258,7 +5264,7 @@
         <v>2001</v>
       </c>
       <c r="D108" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E108"/>
       <c r="F108"/>
@@ -5296,7 +5302,7 @@
         <v>2002</v>
       </c>
       <c r="D109" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E109"/>
       <c r="F109"/>
@@ -5334,7 +5340,7 @@
         <v>2003</v>
       </c>
       <c r="D110" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E110"/>
       <c r="F110"/>
@@ -5372,7 +5378,7 @@
         <v>2004</v>
       </c>
       <c r="D111" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E111"/>
       <c r="F111"/>
@@ -5410,7 +5416,7 @@
         <v>2005</v>
       </c>
       <c r="D112" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E112"/>
       <c r="F112"/>
@@ -5448,7 +5454,7 @@
         <v>2006</v>
       </c>
       <c r="D113" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E113"/>
       <c r="F113"/>
@@ -5465,7 +5471,7 @@
         <v>24</v>
       </c>
       <c r="K113" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L113"/>
       <c r="M113"/>
@@ -5486,7 +5492,7 @@
         <v>2007</v>
       </c>
       <c r="D114" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E114"/>
       <c r="F114"/>
@@ -5524,7 +5530,7 @@
         <v>2008</v>
       </c>
       <c r="D115" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E115"/>
       <c r="F115"/>
@@ -5562,7 +5568,7 @@
         <v>2009</v>
       </c>
       <c r="D116" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E116"/>
       <c r="F116"/>
@@ -5600,7 +5606,7 @@
         <v>2010</v>
       </c>
       <c r="D117" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E117"/>
       <c r="F117"/>
@@ -5638,7 +5644,7 @@
         <v>2011</v>
       </c>
       <c r="D118" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E118"/>
       <c r="F118"/>
@@ -5655,7 +5661,7 @@
         <v>24</v>
       </c>
       <c r="K118" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L118"/>
       <c r="M118"/>
@@ -5676,7 +5682,7 @@
         <v>2012</v>
       </c>
       <c r="D119" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E119"/>
       <c r="F119"/>
@@ -5693,7 +5699,7 @@
         <v>24</v>
       </c>
       <c r="K119" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L119"/>
       <c r="M119"/>
@@ -5714,7 +5720,7 @@
         <v>2013</v>
       </c>
       <c r="D120" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E120"/>
       <c r="F120"/>
@@ -5752,7 +5758,7 @@
         <v>2014</v>
       </c>
       <c r="D121" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E121"/>
       <c r="F121"/>
@@ -5769,7 +5775,7 @@
         <v>24</v>
       </c>
       <c r="K121" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L121"/>
       <c r="M121"/>
@@ -5790,7 +5796,7 @@
         <v>3000</v>
       </c>
       <c r="D122" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E122"/>
       <c r="F122"/>
@@ -5826,7 +5832,7 @@
       </c>
       <c r="C123"/>
       <c r="D123" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E123"/>
       <c r="F123"/>
@@ -5843,7 +5849,7 @@
         <v>24</v>
       </c>
       <c r="K123" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L123"/>
       <c r="M123"/>
@@ -5862,7 +5868,7 @@
       </c>
       <c r="C124"/>
       <c r="D124" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E124"/>
       <c r="F124"/>
@@ -5879,7 +5885,7 @@
         <v>24</v>
       </c>
       <c r="K124" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L124"/>
       <c r="M124"/>
@@ -5898,7 +5904,7 @@
       </c>
       <c r="C125"/>
       <c r="D125" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E125"/>
       <c r="F125"/>
@@ -5915,7 +5921,7 @@
         <v>24</v>
       </c>
       <c r="K125" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L125"/>
       <c r="M125"/>
@@ -5934,7 +5940,7 @@
       </c>
       <c r="C126"/>
       <c r="D126" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E126"/>
       <c r="F126"/>
@@ -5951,7 +5957,7 @@
         <v>24</v>
       </c>
       <c r="K126" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L126"/>
       <c r="M126"/>
@@ -5970,7 +5976,7 @@
       </c>
       <c r="C127"/>
       <c r="D127" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E127"/>
       <c r="F127"/>
@@ -5987,7 +5993,7 @@
         <v>24</v>
       </c>
       <c r="K127" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L127"/>
       <c r="M127"/>
@@ -6006,7 +6012,7 @@
       </c>
       <c r="C128"/>
       <c r="D128" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E128"/>
       <c r="F128"/>
@@ -6023,7 +6029,7 @@
         <v>24</v>
       </c>
       <c r="K128" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L128"/>
       <c r="M128"/>
@@ -6042,7 +6048,7 @@
       </c>
       <c r="C129"/>
       <c r="D129" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E129"/>
       <c r="F129"/>
@@ -6059,7 +6065,7 @@
         <v>24</v>
       </c>
       <c r="K129" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L129"/>
       <c r="M129"/>
@@ -6078,7 +6084,7 @@
       </c>
       <c r="C130"/>
       <c r="D130" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E130"/>
       <c r="F130"/>
@@ -6095,7 +6101,7 @@
         <v>24</v>
       </c>
       <c r="K130" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L130"/>
       <c r="M130"/>
@@ -6114,7 +6120,7 @@
       </c>
       <c r="C131"/>
       <c r="D131" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E131"/>
       <c r="F131"/>
@@ -6131,7 +6137,7 @@
         <v>24</v>
       </c>
       <c r="K131" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="L131"/>
       <c r="M131"/>
@@ -6150,7 +6156,7 @@
       </c>
       <c r="C132"/>
       <c r="D132" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E132"/>
       <c r="F132"/>
@@ -6186,7 +6192,7 @@
       </c>
       <c r="C133"/>
       <c r="D133" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E133"/>
       <c r="F133"/>
@@ -6222,7 +6228,7 @@
       </c>
       <c r="C134"/>
       <c r="D134" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E134"/>
       <c r="F134"/>
@@ -6258,7 +6264,7 @@
       </c>
       <c r="C135"/>
       <c r="D135" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E135"/>
       <c r="F135"/>
@@ -6294,7 +6300,7 @@
       </c>
       <c r="C136"/>
       <c r="D136" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E136"/>
       <c r="F136"/>
@@ -6330,7 +6336,7 @@
       </c>
       <c r="C137"/>
       <c r="D137" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E137"/>
       <c r="F137"/>
@@ -6366,7 +6372,7 @@
       </c>
       <c r="C138"/>
       <c r="D138" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E138"/>
       <c r="F138"/>
@@ -6402,7 +6408,7 @@
       </c>
       <c r="C139"/>
       <c r="D139" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E139"/>
       <c r="F139"/>
@@ -6438,7 +6444,7 @@
       </c>
       <c r="C140"/>
       <c r="D140" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E140"/>
       <c r="F140"/>
@@ -6474,7 +6480,7 @@
       </c>
       <c r="C141"/>
       <c r="D141" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E141"/>
       <c r="F141"/>
@@ -6510,7 +6516,7 @@
       </c>
       <c r="C142"/>
       <c r="D142" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E142"/>
       <c r="F142"/>
@@ -6546,7 +6552,7 @@
       </c>
       <c r="C143"/>
       <c r="D143" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E143"/>
       <c r="F143"/>
@@ -6582,7 +6588,7 @@
       </c>
       <c r="C144"/>
       <c r="D144" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E144"/>
       <c r="F144"/>
@@ -6618,7 +6624,7 @@
       </c>
       <c r="C145"/>
       <c r="D145" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E145"/>
       <c r="F145"/>
@@ -6654,7 +6660,7 @@
       </c>
       <c r="C146"/>
       <c r="D146" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E146"/>
       <c r="F146"/>
@@ -6690,7 +6696,7 @@
       </c>
       <c r="C147"/>
       <c r="D147" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E147"/>
       <c r="F147"/>
@@ -6726,7 +6732,7 @@
       </c>
       <c r="C148"/>
       <c r="D148" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E148"/>
       <c r="F148"/>
@@ -6762,7 +6768,7 @@
       </c>
       <c r="C149"/>
       <c r="D149" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E149"/>
       <c r="F149"/>
@@ -6798,7 +6804,7 @@
       </c>
       <c r="C150"/>
       <c r="D150" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E150"/>
       <c r="F150"/>
@@ -6834,7 +6840,7 @@
       </c>
       <c r="C151"/>
       <c r="D151" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E151"/>
       <c r="F151"/>
@@ -6870,7 +6876,7 @@
       </c>
       <c r="C152"/>
       <c r="D152" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="E152"/>
       <c r="F152"/>
@@ -6906,7 +6912,7 @@
       </c>
       <c r="C153"/>
       <c r="D153" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E153"/>
       <c r="F153"/>
@@ -6942,7 +6948,7 @@
       </c>
       <c r="C154"/>
       <c r="D154" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E154"/>
       <c r="F154"/>
@@ -6978,7 +6984,7 @@
       </c>
       <c r="C155"/>
       <c r="D155" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="E155"/>
       <c r="F155"/>
@@ -7014,7 +7020,7 @@
       </c>
       <c r="C156"/>
       <c r="D156" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E156"/>
       <c r="F156"/>
@@ -7050,7 +7056,7 @@
       </c>
       <c r="C157"/>
       <c r="D157" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E157"/>
       <c r="F157"/>
@@ -7086,7 +7092,7 @@
       </c>
       <c r="C158"/>
       <c r="D158" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E158"/>
       <c r="F158"/>
@@ -7122,7 +7128,7 @@
       </c>
       <c r="C159"/>
       <c r="D159" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E159"/>
       <c r="F159"/>
@@ -7158,7 +7164,7 @@
       </c>
       <c r="C160"/>
       <c r="D160" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E160"/>
       <c r="F160"/>
@@ -7194,7 +7200,7 @@
       </c>
       <c r="C161"/>
       <c r="D161" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E161"/>
       <c r="F161"/>
@@ -7230,7 +7236,7 @@
       </c>
       <c r="C162"/>
       <c r="D162" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="E162"/>
       <c r="F162"/>
@@ -7266,7 +7272,7 @@
       </c>
       <c r="C163"/>
       <c r="D163" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="E163"/>
       <c r="F163"/>
@@ -7302,7 +7308,7 @@
       </c>
       <c r="C164"/>
       <c r="D164" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="E164"/>
       <c r="F164"/>
@@ -7338,7 +7344,7 @@
       </c>
       <c r="C165"/>
       <c r="D165" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="E165"/>
       <c r="F165"/>
@@ -7374,7 +7380,7 @@
       </c>
       <c r="C166"/>
       <c r="D166" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="E166"/>
       <c r="F166"/>
@@ -7410,7 +7416,7 @@
       </c>
       <c r="C167"/>
       <c r="D167" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E167"/>
       <c r="F167"/>
@@ -7448,13 +7454,13 @@
         <v>9535253</v>
       </c>
       <c r="D168" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="E168" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F168" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="G168" t="s">
         <v>21</v>
@@ -7463,10 +7469,10 @@
         <v>22</v>
       </c>
       <c r="I168" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="J168" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="K168" t="s">
         <v>25</v>
@@ -7478,7 +7484,7 @@
       <c r="P168"/>
       <c r="Q168"/>
       <c r="R168" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fitur 2 Tahap ACC Cuti Sama KPI
</commit_message>
<xml_diff>
--- a/assets/excel/Daftar Pegawai.xlsx
+++ b/assets/excel/Daftar Pegawai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="304">
   <si>
     <t>DAFTAR PEGAWAI</t>
   </si>
@@ -95,6 +95,12 @@
     <t>Aktif</t>
   </si>
   <si>
+    <t>SMP</t>
+  </si>
+  <si>
+    <t>0000-00-00</t>
+  </si>
+  <si>
     <t>2012.12.01.003</t>
   </si>
   <si>
@@ -107,6 +113,21 @@
     <t>Iwan Setiyawan</t>
   </si>
   <si>
+    <t>Bantul</t>
+  </si>
+  <si>
+    <t>2022-06-06</t>
+  </si>
+  <si>
+    <t>O-</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>2080-06-06</t>
+  </si>
+  <si>
     <t>2012.12.01.005</t>
   </si>
   <si>
@@ -191,6 +212,9 @@
     <t>Bagus Widodo</t>
   </si>
   <si>
+    <t>D3</t>
+  </si>
+  <si>
     <t>2012.12.01.021</t>
   </si>
   <si>
@@ -827,6 +851,9 @@
     <t>Ihsan Firdaus</t>
   </si>
   <si>
+    <t>DIII</t>
+  </si>
+  <si>
     <t>Arimbi Himsa L</t>
   </si>
   <si>
@@ -890,13 +917,16 @@
     <t>2001-08-09</t>
   </si>
   <si>
-    <t>A-</t>
+    <t>B+</t>
   </si>
   <si>
     <t>Belum Menikah</t>
   </si>
   <si>
-    <t>2059-08-09</t>
+    <t>ratnasari</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
   </si>
 </sst>
 </file>
@@ -1232,7 +1262,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R168"/>
+  <dimension ref="A1:R169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1335,9 +1365,13 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4"/>
-      <c r="P4"/>
+      <c r="P4" t="s">
+        <v>26</v>
+      </c>
       <c r="Q4"/>
-      <c r="R4"/>
+      <c r="R4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5">
@@ -1347,10 +1381,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
@@ -1375,7 +1409,9 @@
       <c r="O5"/>
       <c r="P5"/>
       <c r="Q5"/>
-      <c r="R5"/>
+      <c r="R5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6">
@@ -1385,13 +1421,17 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6"/>
-      <c r="F6"/>
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
       <c r="G6" t="s">
         <v>21</v>
       </c>
@@ -1399,7 +1439,7 @@
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="J6" t="s">
         <v>24</v>
@@ -1411,9 +1451,13 @@
       <c r="M6"/>
       <c r="N6"/>
       <c r="O6"/>
-      <c r="P6"/>
+      <c r="P6" t="s">
+        <v>35</v>
+      </c>
       <c r="Q6"/>
-      <c r="R6"/>
+      <c r="R6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7">
@@ -1423,10 +1467,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E7"/>
       <c r="F7"/>
@@ -1451,7 +1495,9 @@
       <c r="O7"/>
       <c r="P7"/>
       <c r="Q7"/>
-      <c r="R7"/>
+      <c r="R7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8">
@@ -1461,10 +1507,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E8"/>
       <c r="F8"/>
@@ -1489,7 +1535,9 @@
       <c r="O8"/>
       <c r="P8"/>
       <c r="Q8"/>
-      <c r="R8"/>
+      <c r="R8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9">
@@ -1499,10 +1547,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
@@ -1527,7 +1575,9 @@
       <c r="O9"/>
       <c r="P9"/>
       <c r="Q9"/>
-      <c r="R9"/>
+      <c r="R9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10">
@@ -1537,10 +1587,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E10"/>
       <c r="F10"/>
@@ -1565,7 +1615,9 @@
       <c r="O10"/>
       <c r="P10"/>
       <c r="Q10"/>
-      <c r="R10"/>
+      <c r="R10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11">
@@ -1575,10 +1627,10 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E11"/>
       <c r="F11"/>
@@ -1603,7 +1655,9 @@
       <c r="O11"/>
       <c r="P11"/>
       <c r="Q11"/>
-      <c r="R11"/>
+      <c r="R11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12">
@@ -1613,10 +1667,10 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
@@ -1641,7 +1695,9 @@
       <c r="O12"/>
       <c r="P12"/>
       <c r="Q12"/>
-      <c r="R12"/>
+      <c r="R12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13">
@@ -1651,10 +1707,10 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -1679,7 +1735,9 @@
       <c r="O13"/>
       <c r="P13"/>
       <c r="Q13"/>
-      <c r="R13"/>
+      <c r="R13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14">
@@ -1689,10 +1747,10 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -1717,7 +1775,9 @@
       <c r="O14"/>
       <c r="P14"/>
       <c r="Q14"/>
-      <c r="R14"/>
+      <c r="R14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15">
@@ -1727,10 +1787,10 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
@@ -1755,7 +1815,9 @@
       <c r="O15"/>
       <c r="P15"/>
       <c r="Q15"/>
-      <c r="R15"/>
+      <c r="R15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:18">
       <c r="A16">
@@ -1765,10 +1827,10 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
@@ -1793,7 +1855,9 @@
       <c r="O16"/>
       <c r="P16"/>
       <c r="Q16"/>
-      <c r="R16"/>
+      <c r="R16" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" spans="1:18">
       <c r="A17">
@@ -1803,10 +1867,10 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E17"/>
       <c r="F17"/>
@@ -1831,7 +1895,9 @@
       <c r="O17"/>
       <c r="P17"/>
       <c r="Q17"/>
-      <c r="R17"/>
+      <c r="R17" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="1:18">
       <c r="A18">
@@ -1841,10 +1907,10 @@
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
@@ -1869,7 +1935,9 @@
       <c r="O18"/>
       <c r="P18"/>
       <c r="Q18"/>
-      <c r="R18"/>
+      <c r="R18" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="19" spans="1:18">
       <c r="A19">
@@ -1879,10 +1947,10 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
@@ -1907,7 +1975,9 @@
       <c r="O19"/>
       <c r="P19"/>
       <c r="Q19"/>
-      <c r="R19"/>
+      <c r="R19" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20">
@@ -1917,10 +1987,10 @@
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -1943,9 +2013,13 @@
       <c r="M20"/>
       <c r="N20"/>
       <c r="O20"/>
-      <c r="P20"/>
+      <c r="P20" t="s">
+        <v>65</v>
+      </c>
       <c r="Q20"/>
-      <c r="R20"/>
+      <c r="R20" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="21" spans="1:18">
       <c r="A21">
@@ -1955,10 +2029,10 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="E21"/>
       <c r="F21"/>
@@ -1983,7 +2057,9 @@
       <c r="O21"/>
       <c r="P21"/>
       <c r="Q21"/>
-      <c r="R21"/>
+      <c r="R21" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="22" spans="1:18">
       <c r="A22">
@@ -1993,10 +2069,10 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E22"/>
       <c r="F22"/>
@@ -2021,7 +2097,9 @@
       <c r="O22"/>
       <c r="P22"/>
       <c r="Q22"/>
-      <c r="R22"/>
+      <c r="R22" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="23" spans="1:18">
       <c r="A23">
@@ -2031,10 +2109,10 @@
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E23"/>
       <c r="F23"/>
@@ -2059,7 +2137,9 @@
       <c r="O23"/>
       <c r="P23"/>
       <c r="Q23"/>
-      <c r="R23"/>
+      <c r="R23" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:18">
       <c r="A24">
@@ -2069,10 +2149,10 @@
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E24"/>
       <c r="F24"/>
@@ -2097,7 +2177,9 @@
       <c r="O24"/>
       <c r="P24"/>
       <c r="Q24"/>
-      <c r="R24"/>
+      <c r="R24" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:18">
       <c r="A25">
@@ -2107,10 +2189,10 @@
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E25"/>
       <c r="F25"/>
@@ -2135,7 +2217,9 @@
       <c r="O25"/>
       <c r="P25"/>
       <c r="Q25"/>
-      <c r="R25"/>
+      <c r="R25" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26" spans="1:18">
       <c r="A26">
@@ -2145,10 +2229,10 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E26"/>
       <c r="F26"/>
@@ -2173,7 +2257,9 @@
       <c r="O26"/>
       <c r="P26"/>
       <c r="Q26"/>
-      <c r="R26"/>
+      <c r="R26" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" spans="1:18">
       <c r="A27">
@@ -2183,10 +2269,10 @@
         <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E27"/>
       <c r="F27"/>
@@ -2211,7 +2297,9 @@
       <c r="O27"/>
       <c r="P27"/>
       <c r="Q27"/>
-      <c r="R27"/>
+      <c r="R27" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="28" spans="1:18">
       <c r="A28">
@@ -2221,10 +2309,10 @@
         <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E28"/>
       <c r="F28"/>
@@ -2241,7 +2329,7 @@
         <v>24</v>
       </c>
       <c r="K28" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L28"/>
       <c r="M28"/>
@@ -2249,7 +2337,9 @@
       <c r="O28"/>
       <c r="P28"/>
       <c r="Q28"/>
-      <c r="R28"/>
+      <c r="R28" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="29" spans="1:18">
       <c r="A29">
@@ -2259,10 +2349,10 @@
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E29"/>
       <c r="F29"/>
@@ -2287,7 +2377,9 @@
       <c r="O29"/>
       <c r="P29"/>
       <c r="Q29"/>
-      <c r="R29"/>
+      <c r="R29" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="30" spans="1:18">
       <c r="A30">
@@ -2297,10 +2389,10 @@
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="E30"/>
       <c r="F30"/>
@@ -2317,7 +2409,7 @@
         <v>24</v>
       </c>
       <c r="K30" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L30"/>
       <c r="M30"/>
@@ -2325,7 +2417,9 @@
       <c r="O30"/>
       <c r="P30"/>
       <c r="Q30"/>
-      <c r="R30"/>
+      <c r="R30" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="31" spans="1:18">
       <c r="A31">
@@ -2335,10 +2429,10 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E31"/>
       <c r="F31"/>
@@ -2361,9 +2455,13 @@
       <c r="M31"/>
       <c r="N31"/>
       <c r="O31"/>
-      <c r="P31"/>
+      <c r="P31" t="s">
+        <v>35</v>
+      </c>
       <c r="Q31"/>
-      <c r="R31"/>
+      <c r="R31" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="32" spans="1:18">
       <c r="A32">
@@ -2373,10 +2471,10 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E32"/>
       <c r="F32"/>
@@ -2401,7 +2499,9 @@
       <c r="O32"/>
       <c r="P32"/>
       <c r="Q32"/>
-      <c r="R32"/>
+      <c r="R32" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="33" spans="1:18">
       <c r="A33">
@@ -2411,10 +2511,10 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="E33"/>
       <c r="F33"/>
@@ -2439,7 +2539,9 @@
       <c r="O33"/>
       <c r="P33"/>
       <c r="Q33"/>
-      <c r="R33"/>
+      <c r="R33" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="34" spans="1:18">
       <c r="A34">
@@ -2449,10 +2551,10 @@
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E34"/>
       <c r="F34"/>
@@ -2477,7 +2579,9 @@
       <c r="O34"/>
       <c r="P34"/>
       <c r="Q34"/>
-      <c r="R34"/>
+      <c r="R34" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="35" spans="1:18">
       <c r="A35">
@@ -2487,10 +2591,10 @@
         <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E35"/>
       <c r="F35"/>
@@ -2515,7 +2619,9 @@
       <c r="O35"/>
       <c r="P35"/>
       <c r="Q35"/>
-      <c r="R35"/>
+      <c r="R35" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="36" spans="1:18">
       <c r="A36">
@@ -2525,10 +2631,10 @@
         <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E36"/>
       <c r="F36"/>
@@ -2553,7 +2659,9 @@
       <c r="O36"/>
       <c r="P36"/>
       <c r="Q36"/>
-      <c r="R36"/>
+      <c r="R36" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="37" spans="1:18">
       <c r="A37">
@@ -2563,10 +2671,10 @@
         <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E37"/>
       <c r="F37"/>
@@ -2591,7 +2699,9 @@
       <c r="O37"/>
       <c r="P37"/>
       <c r="Q37"/>
-      <c r="R37"/>
+      <c r="R37" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="38" spans="1:18">
       <c r="A38">
@@ -2601,10 +2711,10 @@
         <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D38" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="E38"/>
       <c r="F38"/>
@@ -2629,7 +2739,9 @@
       <c r="O38"/>
       <c r="P38"/>
       <c r="Q38"/>
-      <c r="R38"/>
+      <c r="R38" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="39" spans="1:18">
       <c r="A39">
@@ -2639,10 +2751,10 @@
         <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D39" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E39"/>
       <c r="F39"/>
@@ -2667,7 +2779,9 @@
       <c r="O39"/>
       <c r="P39"/>
       <c r="Q39"/>
-      <c r="R39"/>
+      <c r="R39" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="40" spans="1:18">
       <c r="A40">
@@ -2677,10 +2791,10 @@
         <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E40"/>
       <c r="F40"/>
@@ -2705,7 +2819,9 @@
       <c r="O40"/>
       <c r="P40"/>
       <c r="Q40"/>
-      <c r="R40"/>
+      <c r="R40" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="41" spans="1:18">
       <c r="A41">
@@ -2715,10 +2831,10 @@
         <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D41" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E41"/>
       <c r="F41"/>
@@ -2743,7 +2859,9 @@
       <c r="O41"/>
       <c r="P41"/>
       <c r="Q41"/>
-      <c r="R41"/>
+      <c r="R41" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="42" spans="1:18">
       <c r="A42">
@@ -2753,10 +2871,10 @@
         <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="D42" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E42"/>
       <c r="F42"/>
@@ -2781,7 +2899,9 @@
       <c r="O42"/>
       <c r="P42"/>
       <c r="Q42"/>
-      <c r="R42"/>
+      <c r="R42" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="43" spans="1:18">
       <c r="A43">
@@ -2791,10 +2911,10 @@
         <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="D43" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="E43"/>
       <c r="F43"/>
@@ -2819,7 +2939,9 @@
       <c r="O43"/>
       <c r="P43"/>
       <c r="Q43"/>
-      <c r="R43"/>
+      <c r="R43" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="44" spans="1:18">
       <c r="A44">
@@ -2829,10 +2951,10 @@
         <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D44" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E44"/>
       <c r="F44"/>
@@ -2857,7 +2979,9 @@
       <c r="O44"/>
       <c r="P44"/>
       <c r="Q44"/>
-      <c r="R44"/>
+      <c r="R44" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="45" spans="1:18">
       <c r="A45">
@@ -2867,10 +2991,10 @@
         <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D45" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E45"/>
       <c r="F45"/>
@@ -2895,7 +3019,9 @@
       <c r="O45"/>
       <c r="P45"/>
       <c r="Q45"/>
-      <c r="R45"/>
+      <c r="R45" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="46" spans="1:18">
       <c r="A46">
@@ -2905,10 +3031,10 @@
         <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="D46" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="E46"/>
       <c r="F46"/>
@@ -2933,7 +3059,9 @@
       <c r="O46"/>
       <c r="P46"/>
       <c r="Q46"/>
-      <c r="R46"/>
+      <c r="R46" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="47" spans="1:18">
       <c r="A47">
@@ -2943,10 +3071,10 @@
         <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D47" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="E47"/>
       <c r="F47"/>
@@ -2971,7 +3099,9 @@
       <c r="O47"/>
       <c r="P47"/>
       <c r="Q47"/>
-      <c r="R47"/>
+      <c r="R47" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="48" spans="1:18">
       <c r="A48">
@@ -2981,10 +3111,10 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="D48" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="E48"/>
       <c r="F48"/>
@@ -3009,7 +3139,9 @@
       <c r="O48"/>
       <c r="P48"/>
       <c r="Q48"/>
-      <c r="R48"/>
+      <c r="R48" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="49" spans="1:18">
       <c r="A49">
@@ -3019,10 +3151,10 @@
         <v>46</v>
       </c>
       <c r="C49" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D49" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="E49"/>
       <c r="F49"/>
@@ -3047,7 +3179,9 @@
       <c r="O49"/>
       <c r="P49"/>
       <c r="Q49"/>
-      <c r="R49"/>
+      <c r="R49" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="50" spans="1:18">
       <c r="A50">
@@ -3057,10 +3191,10 @@
         <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D50" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="E50"/>
       <c r="F50"/>
@@ -3085,7 +3219,9 @@
       <c r="O50"/>
       <c r="P50"/>
       <c r="Q50"/>
-      <c r="R50"/>
+      <c r="R50" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="51" spans="1:18">
       <c r="A51">
@@ -3095,10 +3231,10 @@
         <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D51" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="E51"/>
       <c r="F51"/>
@@ -3123,7 +3259,9 @@
       <c r="O51"/>
       <c r="P51"/>
       <c r="Q51"/>
-      <c r="R51"/>
+      <c r="R51" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="52" spans="1:18">
       <c r="A52">
@@ -3133,10 +3271,10 @@
         <v>49</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="D52" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="E52"/>
       <c r="F52"/>
@@ -3161,7 +3299,9 @@
       <c r="O52"/>
       <c r="P52"/>
       <c r="Q52"/>
-      <c r="R52"/>
+      <c r="R52" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="53" spans="1:18">
       <c r="A53">
@@ -3171,10 +3311,10 @@
         <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D53" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="E53"/>
       <c r="F53"/>
@@ -3199,7 +3339,9 @@
       <c r="O53"/>
       <c r="P53"/>
       <c r="Q53"/>
-      <c r="R53"/>
+      <c r="R53" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="54" spans="1:18">
       <c r="A54">
@@ -3209,10 +3351,10 @@
         <v>51</v>
       </c>
       <c r="C54" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D54" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="E54"/>
       <c r="F54"/>
@@ -3237,7 +3379,9 @@
       <c r="O54"/>
       <c r="P54"/>
       <c r="Q54"/>
-      <c r="R54"/>
+      <c r="R54" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="55" spans="1:18">
       <c r="A55">
@@ -3247,10 +3391,10 @@
         <v>52</v>
       </c>
       <c r="C55" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D55" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E55"/>
       <c r="F55"/>
@@ -3267,7 +3411,7 @@
         <v>24</v>
       </c>
       <c r="K55" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L55"/>
       <c r="M55"/>
@@ -3275,7 +3419,9 @@
       <c r="O55"/>
       <c r="P55"/>
       <c r="Q55"/>
-      <c r="R55"/>
+      <c r="R55" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="56" spans="1:18">
       <c r="A56">
@@ -3285,10 +3431,10 @@
         <v>53</v>
       </c>
       <c r="C56" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="D56" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="E56"/>
       <c r="F56"/>
@@ -3313,7 +3459,9 @@
       <c r="O56"/>
       <c r="P56"/>
       <c r="Q56"/>
-      <c r="R56"/>
+      <c r="R56" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="57" spans="1:18">
       <c r="A57">
@@ -3323,10 +3471,10 @@
         <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="D57" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E57"/>
       <c r="F57"/>
@@ -3351,7 +3499,9 @@
       <c r="O57"/>
       <c r="P57"/>
       <c r="Q57"/>
-      <c r="R57"/>
+      <c r="R57" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="58" spans="1:18">
       <c r="A58">
@@ -3361,10 +3511,10 @@
         <v>55</v>
       </c>
       <c r="C58" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D58" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="E58"/>
       <c r="F58"/>
@@ -3389,7 +3539,9 @@
       <c r="O58"/>
       <c r="P58"/>
       <c r="Q58"/>
-      <c r="R58"/>
+      <c r="R58" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="59" spans="1:18">
       <c r="A59">
@@ -3399,10 +3551,10 @@
         <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D59" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E59"/>
       <c r="F59"/>
@@ -3427,7 +3579,9 @@
       <c r="O59"/>
       <c r="P59"/>
       <c r="Q59"/>
-      <c r="R59"/>
+      <c r="R59" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="60" spans="1:18">
       <c r="A60">
@@ -3437,10 +3591,10 @@
         <v>57</v>
       </c>
       <c r="C60" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="D60" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="E60"/>
       <c r="F60"/>
@@ -3465,7 +3619,9 @@
       <c r="O60"/>
       <c r="P60"/>
       <c r="Q60"/>
-      <c r="R60"/>
+      <c r="R60" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="61" spans="1:18">
       <c r="A61">
@@ -3475,10 +3631,10 @@
         <v>58</v>
       </c>
       <c r="C61" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="D61" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="E61"/>
       <c r="F61"/>
@@ -3503,7 +3659,9 @@
       <c r="O61"/>
       <c r="P61"/>
       <c r="Q61"/>
-      <c r="R61"/>
+      <c r="R61" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="62" spans="1:18">
       <c r="A62">
@@ -3513,10 +3671,10 @@
         <v>59</v>
       </c>
       <c r="C62" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D62" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="E62"/>
       <c r="F62"/>
@@ -3541,7 +3699,9 @@
       <c r="O62"/>
       <c r="P62"/>
       <c r="Q62"/>
-      <c r="R62"/>
+      <c r="R62" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="63" spans="1:18">
       <c r="A63">
@@ -3551,10 +3711,10 @@
         <v>60</v>
       </c>
       <c r="C63" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="E63"/>
       <c r="F63"/>
@@ -3571,7 +3731,7 @@
         <v>24</v>
       </c>
       <c r="K63" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L63"/>
       <c r="M63"/>
@@ -3579,7 +3739,9 @@
       <c r="O63"/>
       <c r="P63"/>
       <c r="Q63"/>
-      <c r="R63"/>
+      <c r="R63" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="64" spans="1:18">
       <c r="A64">
@@ -3589,10 +3751,10 @@
         <v>61</v>
       </c>
       <c r="C64" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D64" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E64"/>
       <c r="F64"/>
@@ -3617,7 +3779,9 @@
       <c r="O64"/>
       <c r="P64"/>
       <c r="Q64"/>
-      <c r="R64"/>
+      <c r="R64" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="65" spans="1:18">
       <c r="A65">
@@ -3627,10 +3791,10 @@
         <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D65" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E65"/>
       <c r="F65"/>
@@ -3655,7 +3819,9 @@
       <c r="O65"/>
       <c r="P65"/>
       <c r="Q65"/>
-      <c r="R65"/>
+      <c r="R65" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="66" spans="1:18">
       <c r="A66">
@@ -3665,10 +3831,10 @@
         <v>63</v>
       </c>
       <c r="C66" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D66" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="E66"/>
       <c r="F66"/>
@@ -3693,7 +3859,9 @@
       <c r="O66"/>
       <c r="P66"/>
       <c r="Q66"/>
-      <c r="R66"/>
+      <c r="R66" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="67" spans="1:18">
       <c r="A67">
@@ -3703,10 +3871,10 @@
         <v>64</v>
       </c>
       <c r="C67" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D67" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="E67"/>
       <c r="F67"/>
@@ -3731,7 +3899,9 @@
       <c r="O67"/>
       <c r="P67"/>
       <c r="Q67"/>
-      <c r="R67"/>
+      <c r="R67" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="68" spans="1:18">
       <c r="A68">
@@ -3741,10 +3911,10 @@
         <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D68" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="E68"/>
       <c r="F68"/>
@@ -3769,7 +3939,9 @@
       <c r="O68"/>
       <c r="P68"/>
       <c r="Q68"/>
-      <c r="R68"/>
+      <c r="R68" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="69" spans="1:18">
       <c r="A69">
@@ -3779,10 +3951,10 @@
         <v>66</v>
       </c>
       <c r="C69" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D69" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E69"/>
       <c r="F69"/>
@@ -3807,7 +3979,9 @@
       <c r="O69"/>
       <c r="P69"/>
       <c r="Q69"/>
-      <c r="R69"/>
+      <c r="R69" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="70" spans="1:18">
       <c r="A70">
@@ -3817,10 +3991,10 @@
         <v>67</v>
       </c>
       <c r="C70" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="D70" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="E70"/>
       <c r="F70"/>
@@ -3845,7 +4019,9 @@
       <c r="O70"/>
       <c r="P70"/>
       <c r="Q70"/>
-      <c r="R70"/>
+      <c r="R70" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="71" spans="1:18">
       <c r="A71">
@@ -3855,10 +4031,10 @@
         <v>68</v>
       </c>
       <c r="C71" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D71" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="E71"/>
       <c r="F71"/>
@@ -3883,7 +4059,9 @@
       <c r="O71"/>
       <c r="P71"/>
       <c r="Q71"/>
-      <c r="R71"/>
+      <c r="R71" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="72" spans="1:18">
       <c r="A72">
@@ -3893,10 +4071,10 @@
         <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D72" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E72"/>
       <c r="F72"/>
@@ -3921,7 +4099,9 @@
       <c r="O72"/>
       <c r="P72"/>
       <c r="Q72"/>
-      <c r="R72"/>
+      <c r="R72" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="73" spans="1:18">
       <c r="A73">
@@ -3931,10 +4111,10 @@
         <v>70</v>
       </c>
       <c r="C73" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D73" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="E73"/>
       <c r="F73"/>
@@ -3951,7 +4131,7 @@
         <v>24</v>
       </c>
       <c r="K73" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L73"/>
       <c r="M73"/>
@@ -3959,7 +4139,9 @@
       <c r="O73"/>
       <c r="P73"/>
       <c r="Q73"/>
-      <c r="R73"/>
+      <c r="R73" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="74" spans="1:18">
       <c r="A74">
@@ -3969,10 +4151,10 @@
         <v>71</v>
       </c>
       <c r="C74" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="D74" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="E74"/>
       <c r="F74"/>
@@ -3997,7 +4179,9 @@
       <c r="O74"/>
       <c r="P74"/>
       <c r="Q74"/>
-      <c r="R74"/>
+      <c r="R74" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="75" spans="1:18">
       <c r="A75">
@@ -4007,10 +4191,10 @@
         <v>72</v>
       </c>
       <c r="C75" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D75" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="E75"/>
       <c r="F75"/>
@@ -4027,7 +4211,7 @@
         <v>24</v>
       </c>
       <c r="K75" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L75"/>
       <c r="M75"/>
@@ -4035,7 +4219,9 @@
       <c r="O75"/>
       <c r="P75"/>
       <c r="Q75"/>
-      <c r="R75"/>
+      <c r="R75" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="76" spans="1:18">
       <c r="A76">
@@ -4045,10 +4231,10 @@
         <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="D76" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="E76"/>
       <c r="F76"/>
@@ -4065,7 +4251,7 @@
         <v>24</v>
       </c>
       <c r="K76" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L76"/>
       <c r="M76"/>
@@ -4073,7 +4259,9 @@
       <c r="O76"/>
       <c r="P76"/>
       <c r="Q76"/>
-      <c r="R76"/>
+      <c r="R76" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="77" spans="1:18">
       <c r="A77">
@@ -4083,10 +4271,10 @@
         <v>74</v>
       </c>
       <c r="C77" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D77" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E77"/>
       <c r="F77"/>
@@ -4103,7 +4291,7 @@
         <v>24</v>
       </c>
       <c r="K77" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L77"/>
       <c r="M77"/>
@@ -4111,7 +4299,9 @@
       <c r="O77"/>
       <c r="P77"/>
       <c r="Q77"/>
-      <c r="R77"/>
+      <c r="R77" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="78" spans="1:18">
       <c r="A78">
@@ -4121,10 +4311,10 @@
         <v>75</v>
       </c>
       <c r="C78" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D78" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="E78"/>
       <c r="F78"/>
@@ -4149,7 +4339,9 @@
       <c r="O78"/>
       <c r="P78"/>
       <c r="Q78"/>
-      <c r="R78"/>
+      <c r="R78" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="79" spans="1:18">
       <c r="A79">
@@ -4159,10 +4351,10 @@
         <v>76</v>
       </c>
       <c r="C79" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D79" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E79"/>
       <c r="F79"/>
@@ -4187,7 +4379,9 @@
       <c r="O79"/>
       <c r="P79"/>
       <c r="Q79"/>
-      <c r="R79"/>
+      <c r="R79" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="80" spans="1:18">
       <c r="A80">
@@ -4197,10 +4391,10 @@
         <v>77</v>
       </c>
       <c r="C80" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D80" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="E80"/>
       <c r="F80"/>
@@ -4225,7 +4419,9 @@
       <c r="O80"/>
       <c r="P80"/>
       <c r="Q80"/>
-      <c r="R80"/>
+      <c r="R80" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="81" spans="1:18">
       <c r="A81">
@@ -4235,10 +4431,10 @@
         <v>78</v>
       </c>
       <c r="C81" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="D81" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="E81"/>
       <c r="F81"/>
@@ -4263,7 +4459,9 @@
       <c r="O81"/>
       <c r="P81"/>
       <c r="Q81"/>
-      <c r="R81"/>
+      <c r="R81" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="82" spans="1:18">
       <c r="A82">
@@ -4273,10 +4471,10 @@
         <v>79</v>
       </c>
       <c r="C82" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D82" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E82"/>
       <c r="F82"/>
@@ -4293,7 +4491,7 @@
         <v>24</v>
       </c>
       <c r="K82" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L82"/>
       <c r="M82"/>
@@ -4301,7 +4499,9 @@
       <c r="O82"/>
       <c r="P82"/>
       <c r="Q82"/>
-      <c r="R82"/>
+      <c r="R82" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="83" spans="1:18">
       <c r="A83">
@@ -4311,10 +4511,10 @@
         <v>80</v>
       </c>
       <c r="C83" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="D83" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="E83"/>
       <c r="F83"/>
@@ -4339,7 +4539,9 @@
       <c r="O83"/>
       <c r="P83"/>
       <c r="Q83"/>
-      <c r="R83"/>
+      <c r="R83" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="84" spans="1:18">
       <c r="A84">
@@ -4349,10 +4551,10 @@
         <v>81</v>
       </c>
       <c r="C84" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D84" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="E84"/>
       <c r="F84"/>
@@ -4369,7 +4571,7 @@
         <v>24</v>
       </c>
       <c r="K84" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L84"/>
       <c r="M84"/>
@@ -4377,7 +4579,9 @@
       <c r="O84"/>
       <c r="P84"/>
       <c r="Q84"/>
-      <c r="R84"/>
+      <c r="R84" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="85" spans="1:18">
       <c r="A85">
@@ -4387,10 +4591,10 @@
         <v>82</v>
       </c>
       <c r="C85" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D85" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="E85"/>
       <c r="F85"/>
@@ -4415,7 +4619,9 @@
       <c r="O85"/>
       <c r="P85"/>
       <c r="Q85"/>
-      <c r="R85"/>
+      <c r="R85" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="86" spans="1:18">
       <c r="A86">
@@ -4425,10 +4631,10 @@
         <v>83</v>
       </c>
       <c r="C86" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D86" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="E86"/>
       <c r="F86"/>
@@ -4445,7 +4651,7 @@
         <v>24</v>
       </c>
       <c r="K86" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L86"/>
       <c r="M86"/>
@@ -4453,7 +4659,9 @@
       <c r="O86"/>
       <c r="P86"/>
       <c r="Q86"/>
-      <c r="R86"/>
+      <c r="R86" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="87" spans="1:18">
       <c r="A87">
@@ -4463,10 +4671,10 @@
         <v>84</v>
       </c>
       <c r="C87" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D87" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="E87"/>
       <c r="F87"/>
@@ -4483,7 +4691,7 @@
         <v>24</v>
       </c>
       <c r="K87" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L87"/>
       <c r="M87"/>
@@ -4491,7 +4699,9 @@
       <c r="O87"/>
       <c r="P87"/>
       <c r="Q87"/>
-      <c r="R87"/>
+      <c r="R87" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="88" spans="1:18">
       <c r="A88">
@@ -4501,10 +4711,10 @@
         <v>85</v>
       </c>
       <c r="C88" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="D88" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="E88"/>
       <c r="F88"/>
@@ -4529,7 +4739,9 @@
       <c r="O88"/>
       <c r="P88"/>
       <c r="Q88"/>
-      <c r="R88"/>
+      <c r="R88" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="89" spans="1:18">
       <c r="A89">
@@ -4539,10 +4751,10 @@
         <v>86</v>
       </c>
       <c r="C89" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="D89" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="E89"/>
       <c r="F89"/>
@@ -4559,7 +4771,7 @@
         <v>24</v>
       </c>
       <c r="K89" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L89"/>
       <c r="M89"/>
@@ -4567,7 +4779,9 @@
       <c r="O89"/>
       <c r="P89"/>
       <c r="Q89"/>
-      <c r="R89"/>
+      <c r="R89" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="90" spans="1:18">
       <c r="A90">
@@ -4577,10 +4791,10 @@
         <v>87</v>
       </c>
       <c r="C90" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="D90" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="E90"/>
       <c r="F90"/>
@@ -4605,7 +4819,9 @@
       <c r="O90"/>
       <c r="P90"/>
       <c r="Q90"/>
-      <c r="R90"/>
+      <c r="R90" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="91" spans="1:18">
       <c r="A91">
@@ -4615,10 +4831,10 @@
         <v>88</v>
       </c>
       <c r="C91" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="D91" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="E91"/>
       <c r="F91"/>
@@ -4643,7 +4859,9 @@
       <c r="O91"/>
       <c r="P91"/>
       <c r="Q91"/>
-      <c r="R91"/>
+      <c r="R91" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="92" spans="1:18">
       <c r="A92">
@@ -4653,10 +4871,10 @@
         <v>89</v>
       </c>
       <c r="C92" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="D92" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="E92"/>
       <c r="F92"/>
@@ -4681,7 +4899,9 @@
       <c r="O92"/>
       <c r="P92"/>
       <c r="Q92"/>
-      <c r="R92"/>
+      <c r="R92" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="93" spans="1:18">
       <c r="A93">
@@ -4691,10 +4911,10 @@
         <v>90</v>
       </c>
       <c r="C93" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="D93" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="E93"/>
       <c r="F93"/>
@@ -4711,7 +4931,7 @@
         <v>24</v>
       </c>
       <c r="K93" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L93"/>
       <c r="M93"/>
@@ -4719,7 +4939,9 @@
       <c r="O93"/>
       <c r="P93"/>
       <c r="Q93"/>
-      <c r="R93"/>
+      <c r="R93" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="94" spans="1:18">
       <c r="A94">
@@ -4729,10 +4951,10 @@
         <v>91</v>
       </c>
       <c r="C94" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="D94" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E94"/>
       <c r="F94"/>
@@ -4757,7 +4979,9 @@
       <c r="O94"/>
       <c r="P94"/>
       <c r="Q94"/>
-      <c r="R94"/>
+      <c r="R94" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="95" spans="1:18">
       <c r="A95">
@@ -4767,10 +4991,10 @@
         <v>92</v>
       </c>
       <c r="C95" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D95" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="E95"/>
       <c r="F95"/>
@@ -4787,7 +5011,7 @@
         <v>24</v>
       </c>
       <c r="K95" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L95"/>
       <c r="M95"/>
@@ -4795,7 +5019,9 @@
       <c r="O95"/>
       <c r="P95"/>
       <c r="Q95"/>
-      <c r="R95"/>
+      <c r="R95" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="96" spans="1:18">
       <c r="A96">
@@ -4805,10 +5031,10 @@
         <v>93</v>
       </c>
       <c r="C96" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="D96" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="E96"/>
       <c r="F96"/>
@@ -4833,7 +5059,9 @@
       <c r="O96"/>
       <c r="P96"/>
       <c r="Q96"/>
-      <c r="R96"/>
+      <c r="R96" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="97" spans="1:18">
       <c r="A97">
@@ -4843,10 +5071,10 @@
         <v>94</v>
       </c>
       <c r="C97" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D97" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="E97"/>
       <c r="F97"/>
@@ -4871,7 +5099,9 @@
       <c r="O97"/>
       <c r="P97"/>
       <c r="Q97"/>
-      <c r="R97"/>
+      <c r="R97" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="98" spans="1:18">
       <c r="A98">
@@ -4881,10 +5111,10 @@
         <v>95</v>
       </c>
       <c r="C98" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="D98" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="E98"/>
       <c r="F98"/>
@@ -4909,7 +5139,9 @@
       <c r="O98"/>
       <c r="P98"/>
       <c r="Q98"/>
-      <c r="R98"/>
+      <c r="R98" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="99" spans="1:18">
       <c r="A99">
@@ -4919,10 +5151,10 @@
         <v>96</v>
       </c>
       <c r="C99" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="D99" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="E99"/>
       <c r="F99"/>
@@ -4947,7 +5179,9 @@
       <c r="O99"/>
       <c r="P99"/>
       <c r="Q99"/>
-      <c r="R99"/>
+      <c r="R99" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="100" spans="1:18">
       <c r="A100">
@@ -4957,10 +5191,10 @@
         <v>97</v>
       </c>
       <c r="C100" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="D100" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="E100"/>
       <c r="F100"/>
@@ -4985,7 +5219,9 @@
       <c r="O100"/>
       <c r="P100"/>
       <c r="Q100"/>
-      <c r="R100"/>
+      <c r="R100" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="101" spans="1:18">
       <c r="A101">
@@ -4995,10 +5231,10 @@
         <v>98</v>
       </c>
       <c r="C101" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="D101" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="E101"/>
       <c r="F101"/>
@@ -5023,7 +5259,9 @@
       <c r="O101"/>
       <c r="P101"/>
       <c r="Q101"/>
-      <c r="R101"/>
+      <c r="R101" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="102" spans="1:18">
       <c r="A102">
@@ -5033,10 +5271,10 @@
         <v>99</v>
       </c>
       <c r="C102" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="D102" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="E102"/>
       <c r="F102"/>
@@ -5061,7 +5299,9 @@
       <c r="O102"/>
       <c r="P102"/>
       <c r="Q102"/>
-      <c r="R102"/>
+      <c r="R102" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="103" spans="1:18">
       <c r="A103">
@@ -5074,7 +5314,7 @@
         <v>1000</v>
       </c>
       <c r="D103" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="E103"/>
       <c r="F103"/>
@@ -5091,7 +5331,7 @@
         <v>24</v>
       </c>
       <c r="K103" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="L103"/>
       <c r="M103"/>
@@ -5099,7 +5339,9 @@
       <c r="O103"/>
       <c r="P103"/>
       <c r="Q103"/>
-      <c r="R103"/>
+      <c r="R103" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="104" spans="1:18">
       <c r="A104">
@@ -5112,7 +5354,7 @@
         <v>1001</v>
       </c>
       <c r="D104" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="E104"/>
       <c r="F104"/>
@@ -5129,7 +5371,7 @@
         <v>24</v>
       </c>
       <c r="K104" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="L104"/>
       <c r="M104"/>
@@ -5137,7 +5379,9 @@
       <c r="O104"/>
       <c r="P104"/>
       <c r="Q104"/>
-      <c r="R104"/>
+      <c r="R104" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="105" spans="1:18">
       <c r="A105">
@@ -5150,7 +5394,7 @@
         <v>1002</v>
       </c>
       <c r="D105" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="E105"/>
       <c r="F105"/>
@@ -5175,7 +5419,9 @@
       <c r="O105"/>
       <c r="P105"/>
       <c r="Q105"/>
-      <c r="R105"/>
+      <c r="R105" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="106" spans="1:18">
       <c r="A106">
@@ -5188,7 +5434,7 @@
         <v>1003</v>
       </c>
       <c r="D106" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="E106"/>
       <c r="F106"/>
@@ -5205,7 +5451,7 @@
         <v>24</v>
       </c>
       <c r="K106" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="L106"/>
       <c r="M106"/>
@@ -5213,7 +5459,9 @@
       <c r="O106"/>
       <c r="P106"/>
       <c r="Q106"/>
-      <c r="R106"/>
+      <c r="R106" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="107" spans="1:18">
       <c r="A107">
@@ -5226,7 +5474,7 @@
         <v>2000</v>
       </c>
       <c r="D107" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="E107"/>
       <c r="F107"/>
@@ -5251,7 +5499,9 @@
       <c r="O107"/>
       <c r="P107"/>
       <c r="Q107"/>
-      <c r="R107"/>
+      <c r="R107" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="108" spans="1:18">
       <c r="A108">
@@ -5264,7 +5514,7 @@
         <v>2001</v>
       </c>
       <c r="D108" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="E108"/>
       <c r="F108"/>
@@ -5289,7 +5539,9 @@
       <c r="O108"/>
       <c r="P108"/>
       <c r="Q108"/>
-      <c r="R108"/>
+      <c r="R108" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="109" spans="1:18">
       <c r="A109">
@@ -5302,7 +5554,7 @@
         <v>2002</v>
       </c>
       <c r="D109" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="E109"/>
       <c r="F109"/>
@@ -5327,7 +5579,9 @@
       <c r="O109"/>
       <c r="P109"/>
       <c r="Q109"/>
-      <c r="R109"/>
+      <c r="R109" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="110" spans="1:18">
       <c r="A110">
@@ -5340,7 +5594,7 @@
         <v>2003</v>
       </c>
       <c r="D110" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="E110"/>
       <c r="F110"/>
@@ -5365,7 +5619,9 @@
       <c r="O110"/>
       <c r="P110"/>
       <c r="Q110"/>
-      <c r="R110"/>
+      <c r="R110" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="111" spans="1:18">
       <c r="A111">
@@ -5378,7 +5634,7 @@
         <v>2004</v>
       </c>
       <c r="D111" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="E111"/>
       <c r="F111"/>
@@ -5403,7 +5659,9 @@
       <c r="O111"/>
       <c r="P111"/>
       <c r="Q111"/>
-      <c r="R111"/>
+      <c r="R111" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="112" spans="1:18">
       <c r="A112">
@@ -5416,7 +5674,7 @@
         <v>2005</v>
       </c>
       <c r="D112" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="E112"/>
       <c r="F112"/>
@@ -5441,7 +5699,9 @@
       <c r="O112"/>
       <c r="P112"/>
       <c r="Q112"/>
-      <c r="R112"/>
+      <c r="R112" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="113" spans="1:18">
       <c r="A113">
@@ -5454,7 +5714,7 @@
         <v>2006</v>
       </c>
       <c r="D113" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="E113"/>
       <c r="F113"/>
@@ -5471,7 +5731,7 @@
         <v>24</v>
       </c>
       <c r="K113" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L113"/>
       <c r="M113"/>
@@ -5479,7 +5739,9 @@
       <c r="O113"/>
       <c r="P113"/>
       <c r="Q113"/>
-      <c r="R113"/>
+      <c r="R113" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="114" spans="1:18">
       <c r="A114">
@@ -5492,7 +5754,7 @@
         <v>2007</v>
       </c>
       <c r="D114" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="E114"/>
       <c r="F114"/>
@@ -5517,7 +5779,9 @@
       <c r="O114"/>
       <c r="P114"/>
       <c r="Q114"/>
-      <c r="R114"/>
+      <c r="R114" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="115" spans="1:18">
       <c r="A115">
@@ -5530,7 +5794,7 @@
         <v>2008</v>
       </c>
       <c r="D115" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="E115"/>
       <c r="F115"/>
@@ -5555,7 +5819,9 @@
       <c r="O115"/>
       <c r="P115"/>
       <c r="Q115"/>
-      <c r="R115"/>
+      <c r="R115" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="116" spans="1:18">
       <c r="A116">
@@ -5568,7 +5834,7 @@
         <v>2009</v>
       </c>
       <c r="D116" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="E116"/>
       <c r="F116"/>
@@ -5593,7 +5859,9 @@
       <c r="O116"/>
       <c r="P116"/>
       <c r="Q116"/>
-      <c r="R116"/>
+      <c r="R116" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="117" spans="1:18">
       <c r="A117">
@@ -5606,7 +5874,7 @@
         <v>2010</v>
       </c>
       <c r="D117" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="E117"/>
       <c r="F117"/>
@@ -5631,7 +5899,9 @@
       <c r="O117"/>
       <c r="P117"/>
       <c r="Q117"/>
-      <c r="R117"/>
+      <c r="R117" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="118" spans="1:18">
       <c r="A118">
@@ -5644,7 +5914,7 @@
         <v>2011</v>
       </c>
       <c r="D118" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="E118"/>
       <c r="F118"/>
@@ -5661,7 +5931,7 @@
         <v>24</v>
       </c>
       <c r="K118" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L118"/>
       <c r="M118"/>
@@ -5669,7 +5939,9 @@
       <c r="O118"/>
       <c r="P118"/>
       <c r="Q118"/>
-      <c r="R118"/>
+      <c r="R118" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="119" spans="1:18">
       <c r="A119">
@@ -5682,7 +5954,7 @@
         <v>2012</v>
       </c>
       <c r="D119" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="E119"/>
       <c r="F119"/>
@@ -5699,7 +5971,7 @@
         <v>24</v>
       </c>
       <c r="K119" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L119"/>
       <c r="M119"/>
@@ -5707,7 +5979,9 @@
       <c r="O119"/>
       <c r="P119"/>
       <c r="Q119"/>
-      <c r="R119"/>
+      <c r="R119" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="120" spans="1:18">
       <c r="A120">
@@ -5720,7 +5994,7 @@
         <v>2013</v>
       </c>
       <c r="D120" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="E120"/>
       <c r="F120"/>
@@ -5745,7 +6019,9 @@
       <c r="O120"/>
       <c r="P120"/>
       <c r="Q120"/>
-      <c r="R120"/>
+      <c r="R120" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="121" spans="1:18">
       <c r="A121">
@@ -5758,7 +6034,7 @@
         <v>2014</v>
       </c>
       <c r="D121" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="E121"/>
       <c r="F121"/>
@@ -5775,7 +6051,7 @@
         <v>24</v>
       </c>
       <c r="K121" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L121"/>
       <c r="M121"/>
@@ -5783,7 +6059,9 @@
       <c r="O121"/>
       <c r="P121"/>
       <c r="Q121"/>
-      <c r="R121"/>
+      <c r="R121" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="122" spans="1:18">
       <c r="A122">
@@ -5796,7 +6074,7 @@
         <v>3000</v>
       </c>
       <c r="D122" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="E122"/>
       <c r="F122"/>
@@ -5821,7 +6099,9 @@
       <c r="O122"/>
       <c r="P122"/>
       <c r="Q122"/>
-      <c r="R122"/>
+      <c r="R122" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="123" spans="1:18">
       <c r="A123">
@@ -5832,7 +6112,7 @@
       </c>
       <c r="C123"/>
       <c r="D123" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="E123"/>
       <c r="F123"/>
@@ -5849,7 +6129,7 @@
         <v>24</v>
       </c>
       <c r="K123" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L123"/>
       <c r="M123"/>
@@ -5857,7 +6137,9 @@
       <c r="O123"/>
       <c r="P123"/>
       <c r="Q123"/>
-      <c r="R123"/>
+      <c r="R123" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="124" spans="1:18">
       <c r="A124">
@@ -5868,7 +6150,7 @@
       </c>
       <c r="C124"/>
       <c r="D124" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="E124"/>
       <c r="F124"/>
@@ -5885,7 +6167,7 @@
         <v>24</v>
       </c>
       <c r="K124" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L124"/>
       <c r="M124"/>
@@ -5893,7 +6175,9 @@
       <c r="O124"/>
       <c r="P124"/>
       <c r="Q124"/>
-      <c r="R124"/>
+      <c r="R124" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="125" spans="1:18">
       <c r="A125">
@@ -5904,7 +6188,7 @@
       </c>
       <c r="C125"/>
       <c r="D125" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="E125"/>
       <c r="F125"/>
@@ -5921,7 +6205,7 @@
         <v>24</v>
       </c>
       <c r="K125" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L125"/>
       <c r="M125"/>
@@ -5929,7 +6213,9 @@
       <c r="O125"/>
       <c r="P125"/>
       <c r="Q125"/>
-      <c r="R125"/>
+      <c r="R125" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="126" spans="1:18">
       <c r="A126">
@@ -5940,7 +6226,7 @@
       </c>
       <c r="C126"/>
       <c r="D126" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="E126"/>
       <c r="F126"/>
@@ -5957,7 +6243,7 @@
         <v>24</v>
       </c>
       <c r="K126" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L126"/>
       <c r="M126"/>
@@ -5965,7 +6251,9 @@
       <c r="O126"/>
       <c r="P126"/>
       <c r="Q126"/>
-      <c r="R126"/>
+      <c r="R126" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="127" spans="1:18">
       <c r="A127">
@@ -5976,7 +6264,7 @@
       </c>
       <c r="C127"/>
       <c r="D127" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="E127"/>
       <c r="F127"/>
@@ -5993,7 +6281,7 @@
         <v>24</v>
       </c>
       <c r="K127" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L127"/>
       <c r="M127"/>
@@ -6001,7 +6289,9 @@
       <c r="O127"/>
       <c r="P127"/>
       <c r="Q127"/>
-      <c r="R127"/>
+      <c r="R127" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="128" spans="1:18">
       <c r="A128">
@@ -6012,7 +6302,7 @@
       </c>
       <c r="C128"/>
       <c r="D128" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="E128"/>
       <c r="F128"/>
@@ -6029,7 +6319,7 @@
         <v>24</v>
       </c>
       <c r="K128" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L128"/>
       <c r="M128"/>
@@ -6037,7 +6327,9 @@
       <c r="O128"/>
       <c r="P128"/>
       <c r="Q128"/>
-      <c r="R128"/>
+      <c r="R128" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="129" spans="1:18">
       <c r="A129">
@@ -6048,7 +6340,7 @@
       </c>
       <c r="C129"/>
       <c r="D129" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="E129"/>
       <c r="F129"/>
@@ -6065,7 +6357,7 @@
         <v>24</v>
       </c>
       <c r="K129" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L129"/>
       <c r="M129"/>
@@ -6073,7 +6365,9 @@
       <c r="O129"/>
       <c r="P129"/>
       <c r="Q129"/>
-      <c r="R129"/>
+      <c r="R129" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="130" spans="1:18">
       <c r="A130">
@@ -6084,7 +6378,7 @@
       </c>
       <c r="C130"/>
       <c r="D130" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="E130"/>
       <c r="F130"/>
@@ -6101,7 +6395,7 @@
         <v>24</v>
       </c>
       <c r="K130" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L130"/>
       <c r="M130"/>
@@ -6109,7 +6403,9 @@
       <c r="O130"/>
       <c r="P130"/>
       <c r="Q130"/>
-      <c r="R130"/>
+      <c r="R130" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="131" spans="1:18">
       <c r="A131">
@@ -6120,7 +6416,7 @@
       </c>
       <c r="C131"/>
       <c r="D131" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="E131"/>
       <c r="F131"/>
@@ -6137,7 +6433,7 @@
         <v>24</v>
       </c>
       <c r="K131" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="L131"/>
       <c r="M131"/>
@@ -6145,7 +6441,9 @@
       <c r="O131"/>
       <c r="P131"/>
       <c r="Q131"/>
-      <c r="R131"/>
+      <c r="R131" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="132" spans="1:18">
       <c r="A132">
@@ -6156,7 +6454,7 @@
       </c>
       <c r="C132"/>
       <c r="D132" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="E132"/>
       <c r="F132"/>
@@ -6181,7 +6479,9 @@
       <c r="O132"/>
       <c r="P132"/>
       <c r="Q132"/>
-      <c r="R132"/>
+      <c r="R132" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="133" spans="1:18">
       <c r="A133">
@@ -6192,7 +6492,7 @@
       </c>
       <c r="C133"/>
       <c r="D133" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="E133"/>
       <c r="F133"/>
@@ -6217,7 +6517,9 @@
       <c r="O133"/>
       <c r="P133"/>
       <c r="Q133"/>
-      <c r="R133"/>
+      <c r="R133" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="134" spans="1:18">
       <c r="A134">
@@ -6228,7 +6530,7 @@
       </c>
       <c r="C134"/>
       <c r="D134" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="E134"/>
       <c r="F134"/>
@@ -6253,7 +6555,9 @@
       <c r="O134"/>
       <c r="P134"/>
       <c r="Q134"/>
-      <c r="R134"/>
+      <c r="R134" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="135" spans="1:18">
       <c r="A135">
@@ -6264,7 +6568,7 @@
       </c>
       <c r="C135"/>
       <c r="D135" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="E135"/>
       <c r="F135"/>
@@ -6289,7 +6593,9 @@
       <c r="O135"/>
       <c r="P135"/>
       <c r="Q135"/>
-      <c r="R135"/>
+      <c r="R135" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="136" spans="1:18">
       <c r="A136">
@@ -6300,7 +6606,7 @@
       </c>
       <c r="C136"/>
       <c r="D136" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="E136"/>
       <c r="F136"/>
@@ -6325,7 +6631,9 @@
       <c r="O136"/>
       <c r="P136"/>
       <c r="Q136"/>
-      <c r="R136"/>
+      <c r="R136" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="137" spans="1:18">
       <c r="A137">
@@ -6336,7 +6644,7 @@
       </c>
       <c r="C137"/>
       <c r="D137" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="E137"/>
       <c r="F137"/>
@@ -6361,7 +6669,9 @@
       <c r="O137"/>
       <c r="P137"/>
       <c r="Q137"/>
-      <c r="R137"/>
+      <c r="R137" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="138" spans="1:18">
       <c r="A138">
@@ -6372,7 +6682,7 @@
       </c>
       <c r="C138"/>
       <c r="D138" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="E138"/>
       <c r="F138"/>
@@ -6397,7 +6707,9 @@
       <c r="O138"/>
       <c r="P138"/>
       <c r="Q138"/>
-      <c r="R138"/>
+      <c r="R138" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="139" spans="1:18">
       <c r="A139">
@@ -6408,7 +6720,7 @@
       </c>
       <c r="C139"/>
       <c r="D139" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E139"/>
       <c r="F139"/>
@@ -6433,7 +6745,9 @@
       <c r="O139"/>
       <c r="P139"/>
       <c r="Q139"/>
-      <c r="R139"/>
+      <c r="R139" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="140" spans="1:18">
       <c r="A140">
@@ -6444,7 +6758,7 @@
       </c>
       <c r="C140"/>
       <c r="D140" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E140"/>
       <c r="F140"/>
@@ -6469,7 +6783,9 @@
       <c r="O140"/>
       <c r="P140"/>
       <c r="Q140"/>
-      <c r="R140"/>
+      <c r="R140" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="141" spans="1:18">
       <c r="A141">
@@ -6480,7 +6796,7 @@
       </c>
       <c r="C141"/>
       <c r="D141" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E141"/>
       <c r="F141"/>
@@ -6505,7 +6821,9 @@
       <c r="O141"/>
       <c r="P141"/>
       <c r="Q141"/>
-      <c r="R141"/>
+      <c r="R141" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="142" spans="1:18">
       <c r="A142">
@@ -6516,7 +6834,7 @@
       </c>
       <c r="C142"/>
       <c r="D142" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="E142"/>
       <c r="F142"/>
@@ -6541,7 +6859,9 @@
       <c r="O142"/>
       <c r="P142"/>
       <c r="Q142"/>
-      <c r="R142"/>
+      <c r="R142" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="143" spans="1:18">
       <c r="A143">
@@ -6552,7 +6872,7 @@
       </c>
       <c r="C143"/>
       <c r="D143" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="E143"/>
       <c r="F143"/>
@@ -6577,7 +6897,9 @@
       <c r="O143"/>
       <c r="P143"/>
       <c r="Q143"/>
-      <c r="R143"/>
+      <c r="R143" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="144" spans="1:18">
       <c r="A144">
@@ -6588,7 +6910,7 @@
       </c>
       <c r="C144"/>
       <c r="D144" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E144"/>
       <c r="F144"/>
@@ -6613,7 +6935,9 @@
       <c r="O144"/>
       <c r="P144"/>
       <c r="Q144"/>
-      <c r="R144"/>
+      <c r="R144" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="145" spans="1:18">
       <c r="A145">
@@ -6624,7 +6948,7 @@
       </c>
       <c r="C145"/>
       <c r="D145" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="E145"/>
       <c r="F145"/>
@@ -6649,7 +6973,9 @@
       <c r="O145"/>
       <c r="P145"/>
       <c r="Q145"/>
-      <c r="R145"/>
+      <c r="R145" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="146" spans="1:18">
       <c r="A146">
@@ -6660,7 +6986,7 @@
       </c>
       <c r="C146"/>
       <c r="D146" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="E146"/>
       <c r="F146"/>
@@ -6685,7 +7011,9 @@
       <c r="O146"/>
       <c r="P146"/>
       <c r="Q146"/>
-      <c r="R146"/>
+      <c r="R146" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="147" spans="1:18">
       <c r="A147">
@@ -6696,7 +7024,7 @@
       </c>
       <c r="C147"/>
       <c r="D147" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="E147"/>
       <c r="F147"/>
@@ -6721,7 +7049,9 @@
       <c r="O147"/>
       <c r="P147"/>
       <c r="Q147"/>
-      <c r="R147"/>
+      <c r="R147" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="148" spans="1:18">
       <c r="A148">
@@ -6732,7 +7062,7 @@
       </c>
       <c r="C148"/>
       <c r="D148" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="E148"/>
       <c r="F148"/>
@@ -6755,9 +7085,13 @@
       <c r="M148"/>
       <c r="N148"/>
       <c r="O148"/>
-      <c r="P148"/>
+      <c r="P148" t="s">
+        <v>278</v>
+      </c>
       <c r="Q148"/>
-      <c r="R148"/>
+      <c r="R148" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="149" spans="1:18">
       <c r="A149">
@@ -6768,7 +7102,7 @@
       </c>
       <c r="C149"/>
       <c r="D149" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="E149"/>
       <c r="F149"/>
@@ -6793,7 +7127,9 @@
       <c r="O149"/>
       <c r="P149"/>
       <c r="Q149"/>
-      <c r="R149"/>
+      <c r="R149" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="150" spans="1:18">
       <c r="A150">
@@ -6804,7 +7140,7 @@
       </c>
       <c r="C150"/>
       <c r="D150" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="E150"/>
       <c r="F150"/>
@@ -6829,7 +7165,9 @@
       <c r="O150"/>
       <c r="P150"/>
       <c r="Q150"/>
-      <c r="R150"/>
+      <c r="R150" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="151" spans="1:18">
       <c r="A151">
@@ -6840,7 +7178,7 @@
       </c>
       <c r="C151"/>
       <c r="D151" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="E151"/>
       <c r="F151"/>
@@ -6865,7 +7203,9 @@
       <c r="O151"/>
       <c r="P151"/>
       <c r="Q151"/>
-      <c r="R151"/>
+      <c r="R151" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="152" spans="1:18">
       <c r="A152">
@@ -6876,7 +7216,7 @@
       </c>
       <c r="C152"/>
       <c r="D152" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="E152"/>
       <c r="F152"/>
@@ -6901,7 +7241,9 @@
       <c r="O152"/>
       <c r="P152"/>
       <c r="Q152"/>
-      <c r="R152"/>
+      <c r="R152" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="153" spans="1:18">
       <c r="A153">
@@ -6912,7 +7254,7 @@
       </c>
       <c r="C153"/>
       <c r="D153" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="E153"/>
       <c r="F153"/>
@@ -6937,7 +7279,9 @@
       <c r="O153"/>
       <c r="P153"/>
       <c r="Q153"/>
-      <c r="R153"/>
+      <c r="R153" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="154" spans="1:18">
       <c r="A154">
@@ -6948,7 +7292,7 @@
       </c>
       <c r="C154"/>
       <c r="D154" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="E154"/>
       <c r="F154"/>
@@ -6973,7 +7317,9 @@
       <c r="O154"/>
       <c r="P154"/>
       <c r="Q154"/>
-      <c r="R154"/>
+      <c r="R154" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="155" spans="1:18">
       <c r="A155">
@@ -6984,7 +7330,7 @@
       </c>
       <c r="C155"/>
       <c r="D155" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E155"/>
       <c r="F155"/>
@@ -7009,7 +7355,9 @@
       <c r="O155"/>
       <c r="P155"/>
       <c r="Q155"/>
-      <c r="R155"/>
+      <c r="R155" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="156" spans="1:18">
       <c r="A156">
@@ -7020,7 +7368,7 @@
       </c>
       <c r="C156"/>
       <c r="D156" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="E156"/>
       <c r="F156"/>
@@ -7045,7 +7393,9 @@
       <c r="O156"/>
       <c r="P156"/>
       <c r="Q156"/>
-      <c r="R156"/>
+      <c r="R156" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="157" spans="1:18">
       <c r="A157">
@@ -7056,7 +7406,7 @@
       </c>
       <c r="C157"/>
       <c r="D157" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="E157"/>
       <c r="F157"/>
@@ -7081,7 +7431,9 @@
       <c r="O157"/>
       <c r="P157"/>
       <c r="Q157"/>
-      <c r="R157"/>
+      <c r="R157" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="158" spans="1:18">
       <c r="A158">
@@ -7092,7 +7444,7 @@
       </c>
       <c r="C158"/>
       <c r="D158" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="E158"/>
       <c r="F158"/>
@@ -7117,7 +7469,9 @@
       <c r="O158"/>
       <c r="P158"/>
       <c r="Q158"/>
-      <c r="R158"/>
+      <c r="R158" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="159" spans="1:18">
       <c r="A159">
@@ -7128,7 +7482,7 @@
       </c>
       <c r="C159"/>
       <c r="D159" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="E159"/>
       <c r="F159"/>
@@ -7153,7 +7507,9 @@
       <c r="O159"/>
       <c r="P159"/>
       <c r="Q159"/>
-      <c r="R159"/>
+      <c r="R159" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="160" spans="1:18">
       <c r="A160">
@@ -7164,7 +7520,7 @@
       </c>
       <c r="C160"/>
       <c r="D160" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="E160"/>
       <c r="F160"/>
@@ -7189,7 +7545,9 @@
       <c r="O160"/>
       <c r="P160"/>
       <c r="Q160"/>
-      <c r="R160"/>
+      <c r="R160" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="161" spans="1:18">
       <c r="A161">
@@ -7200,7 +7558,7 @@
       </c>
       <c r="C161"/>
       <c r="D161" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="E161"/>
       <c r="F161"/>
@@ -7225,7 +7583,9 @@
       <c r="O161"/>
       <c r="P161"/>
       <c r="Q161"/>
-      <c r="R161"/>
+      <c r="R161" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="162" spans="1:18">
       <c r="A162">
@@ -7236,7 +7596,7 @@
       </c>
       <c r="C162"/>
       <c r="D162" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="E162"/>
       <c r="F162"/>
@@ -7261,7 +7621,9 @@
       <c r="O162"/>
       <c r="P162"/>
       <c r="Q162"/>
-      <c r="R162"/>
+      <c r="R162" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="163" spans="1:18">
       <c r="A163">
@@ -7272,7 +7634,7 @@
       </c>
       <c r="C163"/>
       <c r="D163" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="E163"/>
       <c r="F163"/>
@@ -7297,7 +7659,9 @@
       <c r="O163"/>
       <c r="P163"/>
       <c r="Q163"/>
-      <c r="R163"/>
+      <c r="R163" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="164" spans="1:18">
       <c r="A164">
@@ -7308,7 +7672,7 @@
       </c>
       <c r="C164"/>
       <c r="D164" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="E164"/>
       <c r="F164"/>
@@ -7333,7 +7697,9 @@
       <c r="O164"/>
       <c r="P164"/>
       <c r="Q164"/>
-      <c r="R164"/>
+      <c r="R164" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="165" spans="1:18">
       <c r="A165">
@@ -7344,7 +7710,7 @@
       </c>
       <c r="C165"/>
       <c r="D165" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="E165"/>
       <c r="F165"/>
@@ -7369,7 +7735,9 @@
       <c r="O165"/>
       <c r="P165"/>
       <c r="Q165"/>
-      <c r="R165"/>
+      <c r="R165" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="166" spans="1:18">
       <c r="A166">
@@ -7380,7 +7748,7 @@
       </c>
       <c r="C166"/>
       <c r="D166" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="E166"/>
       <c r="F166"/>
@@ -7405,7 +7773,9 @@
       <c r="O166"/>
       <c r="P166"/>
       <c r="Q166"/>
-      <c r="R166"/>
+      <c r="R166" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="167" spans="1:18">
       <c r="A167">
@@ -7416,7 +7786,7 @@
       </c>
       <c r="C167"/>
       <c r="D167" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="E167"/>
       <c r="F167"/>
@@ -7441,7 +7811,9 @@
       <c r="O167"/>
       <c r="P167"/>
       <c r="Q167"/>
-      <c r="R167"/>
+      <c r="R167" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="168" spans="1:18">
       <c r="A168">
@@ -7451,16 +7823,16 @@
         <v>165</v>
       </c>
       <c r="C168">
-        <v>9535253</v>
+        <v>123</v>
       </c>
       <c r="D168" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="E168" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="F168" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="G168" t="s">
         <v>21</v>
@@ -7469,10 +7841,10 @@
         <v>22</v>
       </c>
       <c r="I168" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="J168" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="K168" t="s">
         <v>25</v>
@@ -7483,9 +7855,49 @@
       <c r="O168"/>
       <c r="P168"/>
       <c r="Q168"/>
-      <c r="R168" t="s">
-        <v>293</v>
-      </c>
+      <c r="R168"/>
+    </row>
+    <row r="169" spans="1:18">
+      <c r="A169">
+        <v>166</v>
+      </c>
+      <c r="B169">
+        <v>166</v>
+      </c>
+      <c r="C169">
+        <v>1234</v>
+      </c>
+      <c r="D169" t="s">
+        <v>302</v>
+      </c>
+      <c r="E169" t="s">
+        <v>298</v>
+      </c>
+      <c r="F169" t="s">
+        <v>299</v>
+      </c>
+      <c r="G169" t="s">
+        <v>21</v>
+      </c>
+      <c r="H169" t="s">
+        <v>303</v>
+      </c>
+      <c r="I169" t="s">
+        <v>23</v>
+      </c>
+      <c r="J169" t="s">
+        <v>24</v>
+      </c>
+      <c r="K169" t="s">
+        <v>25</v>
+      </c>
+      <c r="L169"/>
+      <c r="M169"/>
+      <c r="N169"/>
+      <c r="O169"/>
+      <c r="P169"/>
+      <c r="Q169"/>
+      <c r="R169"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
perbaikan cuti, izin, approval
</commit_message>
<xml_diff>
--- a/assets/excel/Daftar Pegawai.xlsx
+++ b/assets/excel/Daftar Pegawai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="295">
   <si>
     <t>DAFTAR PEGAWAI</t>
   </si>
@@ -894,6 +894,9 @@
   </si>
   <si>
     <t>Belum Menikah</t>
+  </si>
+  <si>
+    <t>S3</t>
   </si>
   <si>
     <t>2059-08-09</t>
@@ -7481,10 +7484,12 @@
       <c r="M168"/>
       <c r="N168"/>
       <c r="O168"/>
-      <c r="P168"/>
+      <c r="P168" t="s">
+        <v>293</v>
+      </c>
       <c r="Q168"/>
       <c r="R168" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
perbaikan import data pegawai
</commit_message>
<xml_diff>
--- a/assets/excel/Daftar Pegawai.xlsx
+++ b/assets/excel/Daftar Pegawai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="754">
   <si>
     <t>DAFTAR PEGAWAI</t>
   </si>
@@ -80,7 +80,7 @@
     <t>Didik Sudjarwo, SE</t>
   </si>
   <si>
-    <t>2022-07-21</t>
+    <t>2022-07-22</t>
   </si>
   <si>
     <t>Islam</t>
@@ -2277,21 +2277,6 @@
   </si>
   <si>
     <t>087713300137</t>
-  </si>
-  <si>
-    <t>2012.22.07.178</t>
-  </si>
-  <si>
-    <t>Burhanu Sultan Ramadan</t>
-  </si>
-  <si>
-    <t>Darit</t>
-  </si>
-  <si>
-    <t>2001-08-09</t>
-  </si>
-  <si>
-    <t>2059-08-09</t>
   </si>
 </sst>
 </file>
@@ -2627,7 +2612,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R191"/>
+  <dimension ref="A1:R190"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -10891,50 +10876,6 @@
       <c r="P190"/>
       <c r="Q190"/>
       <c r="R190"/>
-    </row>
-    <row r="191" spans="1:18">
-      <c r="A191">
-        <v>188</v>
-      </c>
-      <c r="B191">
-        <v>188</v>
-      </c>
-      <c r="C191" t="s">
-        <v>754</v>
-      </c>
-      <c r="D191" t="s">
-        <v>755</v>
-      </c>
-      <c r="E191" t="s">
-        <v>756</v>
-      </c>
-      <c r="F191" t="s">
-        <v>757</v>
-      </c>
-      <c r="G191" t="s">
-        <v>22</v>
-      </c>
-      <c r="H191" t="s">
-        <v>23</v>
-      </c>
-      <c r="I191" t="s">
-        <v>24</v>
-      </c>
-      <c r="J191" t="s">
-        <v>100</v>
-      </c>
-      <c r="K191" t="s">
-        <v>33</v>
-      </c>
-      <c r="L191"/>
-      <c r="M191"/>
-      <c r="N191"/>
-      <c r="O191"/>
-      <c r="P191"/>
-      <c r="Q191"/>
-      <c r="R191" t="s">
-        <v>758</v>
-      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>